<commit_message>
adding foaf and vcard classes for orgs
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="533">
   <si>
     <t>Requirement</t>
   </si>
@@ -1310,9 +1310,6 @@
   </si>
   <si>
     <t>should be foaf:Organization, should be foaf:member</t>
-  </si>
-  <si>
-    <t>should ne vivo:Department. Should be part of (BFO_0000050 -&gt; we can create hasDepartment be subclassOf of partOt)</t>
   </si>
   <si>
     <t>should be vcard:postal-code</t>
@@ -1581,6 +1578,72 @@
       </rPr>
       <t xml:space="preserve">  hasContact, Person</t>
     </r>
+  </si>
+  <si>
+    <t>Person, hasAddress, Address</t>
+  </si>
+  <si>
+    <t>p34</t>
+  </si>
+  <si>
+    <t>Describing the street address of a person</t>
+  </si>
+  <si>
+    <t>Describing the overall address of a person</t>
+  </si>
+  <si>
+    <t>Address, street address, [string]</t>
+  </si>
+  <si>
+    <t>Describing the locality (city or town) of a person</t>
+  </si>
+  <si>
+    <t>Address, locality, [string]</t>
+  </si>
+  <si>
+    <t>Describing the region (state or province) of a person</t>
+  </si>
+  <si>
+    <t>Address, region, [string]</t>
+  </si>
+  <si>
+    <t>Describing the country of a person</t>
+  </si>
+  <si>
+    <t>Describing the postal code of a person</t>
+  </si>
+  <si>
+    <t>Address, postal code, [string]</t>
+  </si>
+  <si>
+    <t>Address, country name, [string]</t>
+  </si>
+  <si>
+    <t>p35</t>
+  </si>
+  <si>
+    <t>p36</t>
+  </si>
+  <si>
+    <t>p37</t>
+  </si>
+  <si>
+    <t>p38</t>
+  </si>
+  <si>
+    <t>p39</t>
+  </si>
+  <si>
+    <t>REMOVED should ne vivo:Department. Should be part of (BFO_0000050 -&gt; we can create hasDepartment be subclassOf of partOt)</t>
+  </si>
+  <si>
+    <t>O10</t>
+  </si>
+  <si>
+    <t>Describing the parent organization of an organization</t>
+  </si>
+  <si>
+    <t>Organization, isPartOf, Organization</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1821,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1818,13 +1881,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1843,15 +1908,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="59"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="61"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="60"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="62"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="63"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="60"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="59"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="61"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="62"/>
   </cellXfs>
-  <cellStyles count="64">
-    <cellStyle name="Accent2" xfId="63" builtinId="33"/>
-    <cellStyle name="Bad" xfId="61" builtinId="27"/>
+  <cellStyles count="66">
+    <cellStyle name="Accent2" xfId="62" builtinId="33"/>
+    <cellStyle name="Bad" xfId="60" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -1880,7 +1944,10 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="60" builtinId="26"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="59" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1910,8 +1977,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="62" builtinId="28"/>
+    <cellStyle name="Neutral" xfId="61" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
@@ -2252,8 +2318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2267,17 +2333,17 @@
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>505</v>
+      <c r="C1" s="11" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22">
       <c r="B2" s="2"/>
       <c r="C2" s="11" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.5" thickBot="1">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" thickBot="1">
       <c r="A4" t="s">
         <v>312</v>
       </c>
@@ -2291,7 +2357,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" thickTop="1">
+    <row r="5" spans="1:4" ht="17" thickTop="1">
       <c r="A5" t="s">
         <v>313</v>
       </c>
@@ -2302,7 +2368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.5">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" t="s">
         <v>314</v>
       </c>
@@ -2313,7 +2379,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.5">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" t="s">
         <v>315</v>
       </c>
@@ -2324,7 +2390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.5">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" t="s">
         <v>316</v>
       </c>
@@ -2335,7 +2401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.5">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" t="s">
         <v>317</v>
       </c>
@@ -2346,7 +2412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.5">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" t="s">
         <v>318</v>
       </c>
@@ -2357,7 +2423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.5">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" t="s">
         <v>319</v>
       </c>
@@ -2368,7 +2434,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.5">
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -2379,7 +2445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.5">
+    <row r="13" spans="1:4" ht="16">
       <c r="A13" t="s">
         <v>321</v>
       </c>
@@ -2390,7 +2456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.5">
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" t="s">
         <v>322</v>
       </c>
@@ -2401,43 +2467,43 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="11" customFormat="1">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:4" s="10" customFormat="1">
+      <c r="A15" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="11" customFormat="1">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:4" s="10" customFormat="1">
+      <c r="A16" s="10" t="s">
         <v>324</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="11" customFormat="1">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:4" s="10" customFormat="1">
+      <c r="A17" s="10" t="s">
         <v>325</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.5">
+    <row r="18" spans="1:4" ht="16">
       <c r="A18" t="s">
         <v>326</v>
       </c>
@@ -2448,7 +2514,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.5">
+    <row r="19" spans="1:4" ht="16">
       <c r="A19" t="s">
         <v>327</v>
       </c>
@@ -2459,7 +2525,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.5">
+    <row r="20" spans="1:4" ht="16">
       <c r="A20" t="s">
         <v>328</v>
       </c>
@@ -2470,21 +2536,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="12" customFormat="1">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:4" s="11" customFormat="1">
+      <c r="A21" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>511</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17.5">
+    <row r="22" spans="1:4" ht="16">
       <c r="A22" t="s">
         <v>330</v>
       </c>
@@ -2503,10 +2569,10 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.5">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16">
       <c r="A24" t="s">
         <v>332</v>
       </c>
@@ -2517,7 +2583,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.5">
+    <row r="25" spans="1:4" ht="16">
       <c r="A25" t="s">
         <v>333</v>
       </c>
@@ -2528,7 +2594,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.5">
+    <row r="26" spans="1:4" ht="16">
       <c r="A26" t="s">
         <v>334</v>
       </c>
@@ -2539,7 +2605,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.5">
+    <row r="27" spans="1:4" ht="16">
       <c r="A27" t="s">
         <v>335</v>
       </c>
@@ -2561,10 +2627,10 @@
         <v>54</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17.5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16">
       <c r="A29" t="s">
         <v>337</v>
       </c>
@@ -2575,7 +2641,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.5">
+    <row r="30" spans="1:4" ht="16">
       <c r="A30" t="s">
         <v>338</v>
       </c>
@@ -2586,21 +2652,21 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="13" customFormat="1">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:4" s="12" customFormat="1">
+      <c r="A31" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17.5">
+      <c r="D31" s="12" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16">
       <c r="A32" t="s">
         <v>340</v>
       </c>
@@ -2611,7 +2677,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.5">
+    <row r="33" spans="1:4" ht="16">
       <c r="A33" t="s">
         <v>341</v>
       </c>
@@ -2633,7 +2699,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.5">
+    <row r="35" spans="1:4" ht="16">
       <c r="A35" t="s">
         <v>343</v>
       </c>
@@ -2644,7 +2710,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.5">
+    <row r="36" spans="1:4" ht="16">
       <c r="A36" t="s">
         <v>344</v>
       </c>
@@ -2655,35 +2721,35 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="13" customFormat="1">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:4" s="12" customFormat="1">
+      <c r="A37" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="12" customFormat="1">
+      <c r="A38" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="12" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="13" customFormat="1">
-      <c r="A38" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17.5">
+    <row r="39" spans="1:4" ht="16">
       <c r="A39" t="s">
         <v>347</v>
       </c>
@@ -2697,7 +2763,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17.5">
+    <row r="40" spans="1:4" ht="16">
       <c r="A40" t="s">
         <v>348</v>
       </c>
@@ -2711,49 +2777,49 @@
         <v>393</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="11" customFormat="1">
-      <c r="A41" s="11" t="s">
+    <row r="41" spans="1:4" s="10" customFormat="1">
+      <c r="A41" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="11" customFormat="1">
-      <c r="A42" s="11" t="s">
+    <row r="42" spans="1:4" s="10" customFormat="1">
+      <c r="A42" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="11" customFormat="1">
-      <c r="A43" s="11" t="s">
+    <row r="43" spans="1:4" s="10" customFormat="1">
+      <c r="A43" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17.5">
+    <row r="44" spans="1:4" ht="16">
       <c r="A44" t="s">
         <v>352</v>
       </c>
@@ -2767,7 +2833,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17.5">
+    <row r="45" spans="1:4" ht="16">
       <c r="A45" t="s">
         <v>353</v>
       </c>
@@ -2779,7 +2845,7 @@
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" ht="17.5">
+    <row r="46" spans="1:4" ht="16">
       <c r="A46" t="s">
         <v>354</v>
       </c>
@@ -2813,7 +2879,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17.5">
+    <row r="49" spans="1:3" ht="16">
       <c r="A49" t="s">
         <v>357</v>
       </c>
@@ -2824,7 +2890,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="17.5">
+    <row r="50" spans="1:3" ht="16">
       <c r="A50" t="s">
         <v>358</v>
       </c>
@@ -2868,7 +2934,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="17.5">
+    <row r="54" spans="1:3" ht="16">
       <c r="A54" t="s">
         <v>362</v>
       </c>
@@ -2879,7 +2945,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17.5">
+    <row r="55" spans="1:3" ht="16">
       <c r="A55" t="s">
         <v>363</v>
       </c>
@@ -2890,7 +2956,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="17.5">
+    <row r="56" spans="1:3" ht="16">
       <c r="A56" t="s">
         <v>364</v>
       </c>
@@ -2901,7 +2967,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="17.5">
+    <row r="57" spans="1:3" ht="16">
       <c r="A57" t="s">
         <v>365</v>
       </c>
@@ -2912,7 +2978,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="17.5">
+    <row r="58" spans="1:3" ht="16">
       <c r="A58" t="s">
         <v>366</v>
       </c>
@@ -2923,7 +2989,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="17.5">
+    <row r="59" spans="1:3" ht="16">
       <c r="A59" t="s">
         <v>367</v>
       </c>
@@ -2934,7 +3000,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="17.5">
+    <row r="60" spans="1:3" ht="16">
       <c r="A60" t="s">
         <v>368</v>
       </c>
@@ -2945,7 +3011,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="17.5">
+    <row r="61" spans="1:3" ht="16">
       <c r="A61" t="s">
         <v>369</v>
       </c>
@@ -2956,7 +3022,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="17.5">
+    <row r="62" spans="1:3" ht="16">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -2967,7 +3033,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="17.5">
+    <row r="63" spans="1:3" ht="16">
       <c r="A63" t="s">
         <v>371</v>
       </c>
@@ -2978,7 +3044,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="17.5">
+    <row r="64" spans="1:3" ht="16">
       <c r="A64" t="s">
         <v>372</v>
       </c>
@@ -2989,7 +3055,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="17.5">
+    <row r="65" spans="1:3" ht="16">
       <c r="A65" t="s">
         <v>373</v>
       </c>
@@ -3000,7 +3066,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="17.5">
+    <row r="66" spans="1:3" ht="16">
       <c r="A66" t="s">
         <v>374</v>
       </c>
@@ -3011,7 +3077,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="17.5">
+    <row r="67" spans="1:3" ht="16">
       <c r="A67" t="s">
         <v>375</v>
       </c>
@@ -3022,7 +3088,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17.5">
+    <row r="68" spans="1:3" ht="16">
       <c r="A68" t="s">
         <v>376</v>
       </c>
@@ -3033,7 +3099,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.5">
+    <row r="69" spans="1:3" ht="16">
       <c r="A69" t="s">
         <v>377</v>
       </c>
@@ -3044,7 +3110,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17.5">
+    <row r="70" spans="1:3" ht="16">
       <c r="A70" t="s">
         <v>378</v>
       </c>
@@ -3055,7 +3121,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17.5">
+    <row r="71" spans="1:3" ht="16">
       <c r="A71" t="s">
         <v>379</v>
       </c>
@@ -3066,7 +3132,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="17.5">
+    <row r="72" spans="1:3" ht="16">
       <c r="A72" t="s">
         <v>379</v>
       </c>
@@ -3077,7 +3143,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.5">
+    <row r="73" spans="1:3" ht="16">
       <c r="A73" t="s">
         <v>380</v>
       </c>
@@ -3088,7 +3154,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="17.5">
+    <row r="74" spans="1:3" ht="16">
       <c r="A74" t="s">
         <v>381</v>
       </c>
@@ -3099,7 +3165,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="17.5">
+    <row r="75" spans="1:3" ht="16">
       <c r="A75" t="s">
         <v>382</v>
       </c>
@@ -3110,7 +3176,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17.5">
+    <row r="76" spans="1:3" ht="16">
       <c r="A76" t="s">
         <v>383</v>
       </c>
@@ -3121,7 +3187,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="17.5">
+    <row r="77" spans="1:3" ht="16">
       <c r="A77" t="s">
         <v>384</v>
       </c>
@@ -3132,7 +3198,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="17.5">
+    <row r="78" spans="1:3" ht="16">
       <c r="A78" t="s">
         <v>385</v>
       </c>
@@ -3143,7 +3209,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="17.5">
+    <row r="79" spans="1:3" ht="16">
       <c r="A79" t="s">
         <v>386</v>
       </c>
@@ -3154,7 +3220,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="17.5">
+    <row r="80" spans="1:3" ht="16">
       <c r="A80" t="s">
         <v>387</v>
       </c>
@@ -3165,7 +3231,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="17.5">
+    <row r="81" spans="1:3" ht="16">
       <c r="A81" t="s">
         <v>388</v>
       </c>
@@ -3176,7 +3242,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="17.5">
+    <row r="82" spans="1:3" ht="16">
       <c r="A82" t="s">
         <v>389</v>
       </c>
@@ -3212,12 +3278,12 @@
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" t="s">
         <v>312</v>
       </c>
@@ -3231,7 +3297,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" t="s">
         <v>401</v>
       </c>
@@ -3242,7 +3308,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.5">
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" t="s">
         <v>402</v>
       </c>
@@ -3253,7 +3319,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.5">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" t="s">
         <v>403</v>
       </c>
@@ -3264,7 +3330,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.5">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" t="s">
         <v>404</v>
       </c>
@@ -3275,7 +3341,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.5">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" t="s">
         <v>405</v>
       </c>
@@ -3286,7 +3352,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.5">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" t="s">
         <v>406</v>
       </c>
@@ -3297,7 +3363,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.5">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" t="s">
         <v>407</v>
       </c>
@@ -3308,7 +3374,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.5">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" t="s">
         <v>408</v>
       </c>
@@ -3319,7 +3385,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.5">
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" t="s">
         <v>409</v>
       </c>
@@ -3330,7 +3396,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.5">
+    <row r="13" spans="1:4" ht="16">
       <c r="A13" t="s">
         <v>410</v>
       </c>
@@ -3341,7 +3407,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.5">
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" t="s">
         <v>411</v>
       </c>
@@ -3352,7 +3418,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.5">
+    <row r="15" spans="1:4" ht="16">
       <c r="A15" t="s">
         <v>412</v>
       </c>
@@ -3363,7 +3429,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.5">
+    <row r="16" spans="1:4" ht="16">
       <c r="A16" t="s">
         <v>413</v>
       </c>
@@ -3374,7 +3440,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5">
+    <row r="17" spans="1:3" ht="16">
       <c r="A17" t="s">
         <v>414</v>
       </c>
@@ -3385,7 +3451,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.5">
+    <row r="18" spans="1:3" ht="16">
       <c r="A18" t="s">
         <v>415</v>
       </c>
@@ -3396,7 +3462,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.5">
+    <row r="19" spans="1:3" ht="16">
       <c r="A19" t="s">
         <v>416</v>
       </c>
@@ -3407,7 +3473,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.5">
+    <row r="20" spans="1:3" ht="16">
       <c r="A20" t="s">
         <v>417</v>
       </c>
@@ -3418,7 +3484,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.5">
+    <row r="21" spans="1:3" ht="16">
       <c r="A21" t="s">
         <v>418</v>
       </c>
@@ -3429,7 +3495,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.5">
+    <row r="22" spans="1:3" ht="16">
       <c r="A22" t="s">
         <v>419</v>
       </c>
@@ -3440,7 +3506,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17.5">
+    <row r="23" spans="1:3" ht="16">
       <c r="A23" t="s">
         <v>420</v>
       </c>
@@ -3451,7 +3517,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.5">
+    <row r="24" spans="1:3" ht="16">
       <c r="A24" t="s">
         <v>421</v>
       </c>
@@ -3462,7 +3528,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.5">
+    <row r="25" spans="1:3" ht="16">
       <c r="A25" t="s">
         <v>422</v>
       </c>
@@ -3473,7 +3539,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17.5">
+    <row r="26" spans="1:3" ht="16">
       <c r="A26" t="s">
         <v>423</v>
       </c>
@@ -3484,7 +3550,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="17.5">
+    <row r="27" spans="1:3" ht="16">
       <c r="A27" t="s">
         <v>424</v>
       </c>
@@ -3495,7 +3561,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17.5">
+    <row r="28" spans="1:3" ht="16">
       <c r="A28" t="s">
         <v>425</v>
       </c>
@@ -3522,7 +3588,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3531,15 +3597,15 @@
     <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.75">
+    <row r="1" spans="1:5" ht="22">
       <c r="B1" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.5" thickBot="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" thickBot="1">
       <c r="A3" t="s">
         <v>312</v>
       </c>
@@ -3553,9 +3619,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" thickTop="1">
+    <row r="4" spans="1:5" ht="17" thickTop="1">
       <c r="A4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>206</v>
@@ -3567,107 +3633,107 @@
         <v>428</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" s="13" customFormat="1">
+      <c r="A5" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="11" customFormat="1">
+      <c r="A6" s="11" t="s">
         <v>438</v>
       </c>
-      <c r="B5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B6" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="11" customFormat="1">
+      <c r="A7" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="11" customFormat="1">
+      <c r="A8" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="11" customFormat="1">
+      <c r="A9" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="11" customFormat="1">
+      <c r="A10" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="11" customFormat="1">
+      <c r="A11" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>439</v>
-      </c>
-      <c r="B6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D6" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>440</v>
-      </c>
-      <c r="B7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>441</v>
-      </c>
-      <c r="B8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>442</v>
-      </c>
-      <c r="B9" t="s">
-        <v>216</v>
-      </c>
-      <c r="C9" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>443</v>
-      </c>
-      <c r="B10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" t="s">
-        <v>218</v>
-      </c>
-      <c r="D10" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>444</v>
-      </c>
-      <c r="B11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C11" t="s">
-        <v>221</v>
-      </c>
-      <c r="D11" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B12" t="s">
         <v>222</v>
@@ -3679,12 +3745,23 @@
         <v>427</v>
       </c>
       <c r="E12" t="s">
-        <v>508</v>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>530</v>
+      </c>
+      <c r="B13" t="s">
+        <v>531</v>
+      </c>
+      <c r="C13" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -3707,7 +3784,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3717,12 +3794,12 @@
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" t="s">
         <v>312</v>
       </c>
@@ -3736,7 +3813,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" t="s">
         <v>397</v>
       </c>
@@ -3747,10 +3824,10 @@
         <v>226</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.5">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" t="s">
         <v>398</v>
       </c>
@@ -3761,10 +3838,10 @@
         <v>228</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.5">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" t="s">
         <v>399</v>
       </c>
@@ -3776,7 +3853,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="17.5">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" t="s">
         <v>400</v>
       </c>
@@ -3788,9 +3865,9 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="17.5">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>232</v>
@@ -3800,9 +3877,9 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="17.5">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>233</v>
@@ -3812,9 +3889,9 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="17.5">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>234</v>
@@ -3824,9 +3901,9 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="17.5">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>236</v>
@@ -3836,9 +3913,9 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="17.5">
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>240</v>
@@ -3848,9 +3925,9 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" ht="17.5">
+    <row r="13" spans="1:4" ht="16">
       <c r="A13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>243</v>
@@ -3859,26 +3936,26 @@
         <v>244</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.5">
-      <c r="A14" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="13" customFormat="1">
+      <c r="A14" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" t="s">
         <v>452</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17.5">
-      <c r="A15" t="s">
-        <v>453</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>250</v>
@@ -3887,12 +3964,12 @@
         <v>249</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>247</v>
@@ -3901,24 +3978,24 @@
         <v>248</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16">
       <c r="A17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>251</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" ht="16">
       <c r="A18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>252</v>
@@ -3930,7 +4007,7 @@
     </row>
     <row r="19" spans="1:4" ht="16">
       <c r="A19" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>254</v>
@@ -3939,54 +4016,54 @@
         <v>255</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="11" customFormat="1">
-      <c r="A20" s="11" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="10" customFormat="1">
+      <c r="A20" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="10" customFormat="1">
+      <c r="A21" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="B21" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="11" customFormat="1">
-      <c r="A21" s="11" t="s">
+    <row r="22" spans="1:4" s="13" customFormat="1">
+      <c r="A22" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="11" customFormat="1">
-      <c r="A22" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>258</v>
+      <c r="D22" s="13" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16">
       <c r="A23" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>263</v>
@@ -3995,12 +4072,12 @@
         <v>264</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16">
       <c r="A24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>265</v>
@@ -4012,7 +4089,7 @@
     </row>
     <row r="25" spans="1:4" ht="16">
       <c r="A25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>267</v>
@@ -4021,12 +4098,12 @@
         <v>248</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16">
       <c r="A26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>268</v>
@@ -4035,12 +4112,12 @@
         <v>269</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16">
       <c r="A27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>270</v>
@@ -4049,26 +4126,26 @@
         <v>271</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="14" customFormat="1">
-      <c r="A28" s="14" t="s">
-        <v>466</v>
-      </c>
-      <c r="B28" s="14" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="13" customFormat="1">
+      <c r="A28" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>509</v>
+      <c r="D28" s="13" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16">
       <c r="A29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>274</v>
@@ -4077,12 +4154,12 @@
         <v>275</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16">
       <c r="A30" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>276</v>
@@ -4094,7 +4171,7 @@
     </row>
     <row r="31" spans="1:4" ht="16">
       <c r="A31" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>278</v>
@@ -4104,23 +4181,23 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" s="13" customFormat="1">
-      <c r="A32" s="13" t="s">
-        <v>470</v>
-      </c>
-      <c r="B32" s="13" t="s">
+    <row r="32" spans="1:4" s="12" customFormat="1">
+      <c r="A32" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="B32" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>475</v>
+      <c r="D32" s="12" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
       <c r="A33" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>283</v>
@@ -4129,12 +4206,12 @@
         <v>282</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16">
       <c r="A34" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>284</v>
@@ -4143,12 +4220,12 @@
         <v>285</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16">
       <c r="A35" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>286</v>
@@ -4160,7 +4237,7 @@
     </row>
     <row r="36" spans="1:4" ht="16">
       <c r="A36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>288</v>
@@ -4171,21 +4248,75 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="16">
+      <c r="A37" t="s">
+        <v>512</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>511</v>
+      </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="16">
+      <c r="A38" t="s">
+        <v>524</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>515</v>
+      </c>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" ht="16">
+      <c r="A39" t="s">
+        <v>525</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>517</v>
+      </c>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" ht="16">
+      <c r="A40" t="s">
+        <v>526</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>519</v>
+      </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="16">
+      <c r="A41" t="s">
+        <v>527</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>523</v>
+      </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="16">
+      <c r="A42" t="s">
+        <v>528</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>522</v>
+      </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="16">
@@ -4271,12 +4402,12 @@
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4287,9 +4418,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>298</v>
@@ -4299,9 +4430,9 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="17.5">
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>297</v>
@@ -4311,9 +4442,9 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="17.5">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -4323,9 +4454,9 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="17.5">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>300</v>
@@ -4335,9 +4466,9 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="17.5">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>302</v>
@@ -4346,12 +4477,12 @@
         <v>303</v>
       </c>
       <c r="D8" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17.5">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>304</v>
@@ -4360,9 +4491,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.5">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>306</v>
@@ -4371,9 +4502,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.5">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>308</v>
@@ -4382,12 +4513,12 @@
         <v>309</v>
       </c>
       <c r="D11" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.5">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>310</v>
@@ -4396,7 +4527,7 @@
         <v>311</v>
       </c>
       <c r="D12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to organization ontology
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-456" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-456" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="550">
   <si>
     <t>Requirement</t>
   </si>
@@ -658,45 +658,24 @@
     <t>Describing the departments of an organization</t>
   </si>
   <si>
-    <t>Organization, hasDepartment, Department</t>
-  </si>
-  <si>
-    <t>Organization, hasCity, [string]</t>
-  </si>
-  <si>
-    <t>Organization, hasCountry, [string]</t>
-  </si>
-  <si>
     <t>Describing the city in which an organization is located</t>
   </si>
   <si>
     <t>Describing the country in which an organization is located</t>
   </si>
   <si>
-    <t>Organization, hasProvince, [string]</t>
-  </si>
-  <si>
     <t>Describing the province in which an organization is located</t>
   </si>
   <si>
     <t>Describing the state in which an organization is located</t>
   </si>
   <si>
-    <t>Organization, hasState, [string]</t>
-  </si>
-  <si>
-    <t>Organization, hasStreetAddress, [string]</t>
-  </si>
-  <si>
     <t>Describing the street address of an organization</t>
   </si>
   <si>
     <t>Describing the zip or postal code of an organization</t>
   </si>
   <si>
-    <t>Organization, hasZipCode, [string]</t>
-  </si>
-  <si>
     <t>Describing the type of an organization</t>
   </si>
   <si>
@@ -763,9 +742,6 @@
     <t>Describing the degree of a person</t>
   </si>
   <si>
-    <t>Person, hasDegree, Degree</t>
-  </si>
-  <si>
     <t>Describing the department of a person</t>
   </si>
   <si>
@@ -937,9 +913,6 @@
     <t>WorkingGroup, hasWGChair, Person</t>
   </si>
   <si>
-    <t>Describing the MOU of a working group</t>
-  </si>
-  <si>
     <t>WorkingGroup, hasMOU, [string]</t>
   </si>
   <si>
@@ -1309,36 +1282,9 @@
     <t>Pr25</t>
   </si>
   <si>
-    <t xml:space="preserve">Organization, type, {"College" , "Consortium" , "Hospital" , "Institute" , "University"} </t>
-  </si>
-  <si>
-    <t>type is rdf:type</t>
-  </si>
-  <si>
-    <t>should be foaf:Organization, should be foaf:member</t>
-  </si>
-  <si>
-    <t>should be vcard:postal-code</t>
-  </si>
-  <si>
     <t>Most of these can be reused from: https://www.w3.org/TR/vcard-rdf/</t>
   </si>
   <si>
-    <t>http://www.w3.org/2006/vcard/ns#region</t>
-  </si>
-  <si>
-    <t>should be vcard:countryName</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2006/vcard/ns#region why do we need to distinguish between province and state?</t>
-  </si>
-  <si>
-    <t>vcard:locality</t>
-  </si>
-  <si>
-    <t>All the types should be inherited from http://vivoweb.org/ontology/core#</t>
-  </si>
-  <si>
     <t>O1</t>
   </si>
   <si>
@@ -1462,9 +1408,6 @@
     <t>Why not project hasDataAnalyst Person??</t>
   </si>
   <si>
-    <t>This should be a string. Do we have a degree taxonomy?</t>
-  </si>
-  <si>
     <t>Why do we need EnigmaPublication, not just "Publication"?</t>
   </si>
   <si>
@@ -1519,15 +1462,6 @@
     <t>WG9</t>
   </si>
   <si>
-    <t>Why is paper a string? Should it be a DOI? I am confused</t>
-  </si>
-  <si>
-    <t>What is a MOU?</t>
-  </si>
-  <si>
-    <t>This should be just "description"</t>
-  </si>
-  <si>
     <t>CohortGroup, hasFirstDegreeRelativeWithDisorder, Disorder</t>
   </si>
   <si>
@@ -1547,12 +1481,6 @@
   </si>
   <si>
     <t>CLARIFY IF HAS IS THE SAME AS INCLUDES</t>
-  </si>
-  <si>
-    <t>should be vcard:street-address. Need to add address object</t>
-  </si>
-  <si>
-    <t>add department</t>
   </si>
   <si>
     <t>REMOVED</t>
@@ -1640,18 +1568,12 @@
     <t>p39</t>
   </si>
   <si>
-    <t>REMOVED should ne vivo:Department. Should be part of (BFO_0000050 -&gt; we can create hasDepartment be subclassOf of partOt)</t>
-  </si>
-  <si>
     <t>O10</t>
   </si>
   <si>
     <t>Describing the parent organization of an organization</t>
   </si>
   <si>
-    <t>Organization, isPartOf, Organization</t>
-  </si>
-  <si>
     <t>What is the ORCID id of an author?</t>
   </si>
   <si>
@@ -1698,13 +1620,94 @@
   </si>
   <si>
     <t>Which data protocols were run in order to collect a cohort?</t>
+  </si>
+  <si>
+    <t>Describing the Memorandum of understanding of a working group</t>
+  </si>
+  <si>
+    <t>What is the role of a person in an organization?</t>
+  </si>
+  <si>
+    <t>What organizations did a person belong to?</t>
+  </si>
+  <si>
+    <t>What period did a person serve in an organization?</t>
+  </si>
+  <si>
+    <t>What is the primary address of an organization?</t>
+  </si>
+  <si>
+    <t>foaf:Organization. hasAffiliate subclass of foaf:member</t>
+  </si>
+  <si>
+    <t>Organization, isPartOfOrganziation, Department</t>
+  </si>
+  <si>
+    <t>Organization, vcard:hasAddress, Address, vcard:locality, [string]</t>
+  </si>
+  <si>
+    <t>Organization, vcard:hasAddress, vcard:countryName, [string]</t>
+  </si>
+  <si>
+    <t>Organization, vcard:hasAddress, vcard:region, [string]</t>
+  </si>
+  <si>
+    <t>Organization, vcard:hasAddress, vcard:street-address, [string]</t>
+  </si>
+  <si>
+    <t>Organization, vcard:hasAddress, vcard:postalCode, [string]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization, rdf:type, {"College" ,"Center", "Consortium" , "Hospital" , "Institute" , "University", "Department"} </t>
+  </si>
+  <si>
+    <t>SEE also O10</t>
+  </si>
+  <si>
+    <t>SEE also O6</t>
+  </si>
+  <si>
+    <t>Organization, isPartOfOrganization, Organization</t>
+  </si>
+  <si>
+    <t>Add in the def: an organization may be part of more than more organizations.</t>
+  </si>
+  <si>
+    <t>Organization, hasPrimaryAddress, Address</t>
+  </si>
+  <si>
+    <t>Separate to a separate module called ENIGMA roles</t>
+  </si>
+  <si>
+    <t>Person, hasDegree, string</t>
+  </si>
+  <si>
+    <t>Change to string</t>
+  </si>
+  <si>
+    <t>Clarify in the definition</t>
+  </si>
+  <si>
+    <t>This should be Working Group. Should keep description, because they may have 2</t>
+  </si>
+  <si>
+    <t>P40</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>P42</t>
+  </si>
+  <si>
+    <t>P43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1819,16 +1822,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1853,11 +1848,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
   </fills>
@@ -1903,7 +1893,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1970,7 +1960,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1995,12 +1984,11 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="59"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="61"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="62"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="66"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="59" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="66">
     <cellStyle name="Accent2" xfId="62" builtinId="33"/>
     <cellStyle name="Bad" xfId="60" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="66" builtinId="23"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -2419,18 +2407,18 @@
         <v>8</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="11" t="s">
-        <v>505</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2439,12 +2427,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -2455,7 +2443,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>23</v>
@@ -2466,7 +2454,7 @@
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -2477,7 +2465,7 @@
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -2488,7 +2476,7 @@
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>24</v>
@@ -2499,7 +2487,7 @@
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -2510,7 +2498,7 @@
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -2521,7 +2509,7 @@
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
@@ -2532,7 +2520,7 @@
     </row>
     <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>25</v>
@@ -2543,7 +2531,7 @@
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -2554,7 +2542,7 @@
     </row>
     <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>28</v>
@@ -2563,12 +2551,12 @@
         <v>29</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -2579,7 +2567,7 @@
     </row>
     <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>32</v>
@@ -2590,7 +2578,7 @@
     </row>
     <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>34</v>
@@ -2601,7 +2589,7 @@
     </row>
     <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -2612,7 +2600,7 @@
     </row>
     <row r="20" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>38</v>
@@ -2623,21 +2611,21 @@
     </row>
     <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>41</v>
@@ -2648,18 +2636,18 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>47</v>
@@ -2670,7 +2658,7 @@
     </row>
     <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>48</v>
@@ -2681,7 +2669,7 @@
     </row>
     <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>49</v>
@@ -2692,7 +2680,7 @@
     </row>
     <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>51</v>
@@ -2703,7 +2691,7 @@
     </row>
     <row r="28" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>53</v>
@@ -2712,12 +2700,12 @@
         <v>54</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>55</v>
@@ -2728,7 +2716,7 @@
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>57</v>
@@ -2739,7 +2727,7 @@
     </row>
     <row r="31" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>59</v>
@@ -2748,12 +2736,12 @@
         <v>3</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>60</v>
@@ -2764,7 +2752,7 @@
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>62</v>
@@ -2775,7 +2763,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
@@ -2786,7 +2774,7 @@
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>66</v>
@@ -2797,7 +2785,7 @@
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>68</v>
@@ -2808,7 +2796,7 @@
     </row>
     <row r="37" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>70</v>
@@ -2817,12 +2805,12 @@
         <v>71</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>72</v>
@@ -2831,12 +2819,12 @@
         <v>73</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>74</v>
@@ -2845,12 +2833,12 @@
         <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>76</v>
@@ -2859,12 +2847,12 @@
         <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>78</v>
@@ -2873,12 +2861,12 @@
         <v>168</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>79</v>
@@ -2887,12 +2875,12 @@
         <v>169</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>80</v>
@@ -2901,50 +2889,50 @@
         <v>170</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="B47" t="s">
         <v>81</v>
@@ -2955,7 +2943,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="B48" t="s">
         <v>82</v>
@@ -2966,7 +2954,7 @@
     </row>
     <row r="49" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>83</v>
@@ -2977,7 +2965,7 @@
     </row>
     <row r="50" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>84</v>
@@ -2988,7 +2976,7 @@
     </row>
     <row r="51" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>85</v>
@@ -2999,7 +2987,7 @@
     </row>
     <row r="52" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>86</v>
@@ -3010,7 +2998,7 @@
     </row>
     <row r="53" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>87</v>
@@ -3021,7 +3009,7 @@
     </row>
     <row r="54" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>88</v>
@@ -3032,7 +3020,7 @@
     </row>
     <row r="55" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>89</v>
@@ -3043,7 +3031,7 @@
     </row>
     <row r="56" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>90</v>
@@ -3054,7 +3042,7 @@
     </row>
     <row r="57" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>91</v>
@@ -3065,7 +3053,7 @@
     </row>
     <row r="58" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>92</v>
@@ -3076,7 +3064,7 @@
     </row>
     <row r="59" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>93</v>
@@ -3087,7 +3075,7 @@
     </row>
     <row r="60" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>94</v>
@@ -3098,7 +3086,7 @@
     </row>
     <row r="61" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>95</v>
@@ -3109,7 +3097,7 @@
     </row>
     <row r="62" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>96</v>
@@ -3120,7 +3108,7 @@
     </row>
     <row r="63" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>97</v>
@@ -3131,7 +3119,7 @@
     </row>
     <row r="64" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>98</v>
@@ -3142,7 +3130,7 @@
     </row>
     <row r="65" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>99</v>
@@ -3153,7 +3141,7 @@
     </row>
     <row r="66" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>100</v>
@@ -3164,7 +3152,7 @@
     </row>
     <row r="67" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>101</v>
@@ -3175,7 +3163,7 @@
     </row>
     <row r="68" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>102</v>
@@ -3186,7 +3174,7 @@
     </row>
     <row r="69" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>103</v>
@@ -3197,7 +3185,7 @@
     </row>
     <row r="70" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>104</v>
@@ -3208,7 +3196,7 @@
     </row>
     <row r="71" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>105</v>
@@ -3219,7 +3207,7 @@
     </row>
     <row r="72" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>106</v>
@@ -3230,7 +3218,7 @@
     </row>
     <row r="73" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>107</v>
@@ -3241,7 +3229,7 @@
     </row>
     <row r="74" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>108</v>
@@ -3252,7 +3240,7 @@
     </row>
     <row r="75" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>109</v>
@@ -3263,7 +3251,7 @@
     </row>
     <row r="76" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>110</v>
@@ -3274,7 +3262,7 @@
     </row>
     <row r="77" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>111</v>
@@ -3285,7 +3273,7 @@
     </row>
     <row r="78" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>112</v>
@@ -3296,7 +3284,7 @@
     </row>
     <row r="79" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>113</v>
@@ -3307,7 +3295,7 @@
     </row>
     <row r="80" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>114</v>
@@ -3318,7 +3306,7 @@
     </row>
     <row r="81" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>115</v>
@@ -3329,7 +3317,7 @@
     </row>
     <row r="82" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>116</v>
@@ -3340,7 +3328,7 @@
     </row>
     <row r="83" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B83" s="5" t="s">
-        <v>548</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -3358,7 +3346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -3375,7 +3363,7 @@
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3384,12 +3372,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3400,7 +3388,7 @@
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>118</v>
@@ -3411,7 +3399,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>120</v>
@@ -3422,7 +3410,7 @@
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>122</v>
@@ -3433,7 +3421,7 @@
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>124</v>
@@ -3444,7 +3432,7 @@
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>126</v>
@@ -3455,7 +3443,7 @@
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>128</v>
@@ -3466,7 +3454,7 @@
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>130</v>
@@ -3477,7 +3465,7 @@
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>132</v>
@@ -3488,7 +3476,7 @@
     </row>
     <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>134</v>
@@ -3499,7 +3487,7 @@
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>136</v>
@@ -3510,7 +3498,7 @@
     </row>
     <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>138</v>
@@ -3521,7 +3509,7 @@
     </row>
     <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>140</v>
@@ -3532,7 +3520,7 @@
     </row>
     <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>142</v>
@@ -3543,7 +3531,7 @@
     </row>
     <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>144</v>
@@ -3554,7 +3542,7 @@
     </row>
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>147</v>
@@ -3565,7 +3553,7 @@
     </row>
     <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>148</v>
@@ -3576,7 +3564,7 @@
     </row>
     <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>150</v>
@@ -3587,7 +3575,7 @@
     </row>
     <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>152</v>
@@ -3598,7 +3586,7 @@
     </row>
     <row r="23" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>154</v>
@@ -3609,7 +3597,7 @@
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>156</v>
@@ -3620,7 +3608,7 @@
     </row>
     <row r="25" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>158</v>
@@ -3631,7 +3619,7 @@
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>159</v>
@@ -3642,7 +3630,7 @@
     </row>
     <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>161</v>
@@ -3653,7 +3641,7 @@
     </row>
     <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>163</v>
@@ -3675,10 +3663,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3687,17 +3675,17 @@
     <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3706,12 +3694,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>206</v>
@@ -3720,153 +3708,129 @@
         <v>207</v>
       </c>
       <c r="D4" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>437</v>
-      </c>
-      <c r="B5" s="13" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>532</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="C9" s="11" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>440</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>426</v>
+      </c>
+      <c r="B12" t="s">
         <v>215</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="C12" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>505</v>
+      </c>
+      <c r="B13" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>444</v>
-      </c>
-      <c r="B12" t="s">
-        <v>222</v>
-      </c>
-      <c r="C12" t="s">
-        <v>426</v>
-      </c>
-      <c r="D12" t="s">
-        <v>427</v>
-      </c>
-      <c r="E12" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>530</v>
-      </c>
-      <c r="B13" t="s">
-        <v>531</v>
-      </c>
       <c r="C13" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>538</v>
+      </c>
+      <c r="D13" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>534</v>
+        <v>508</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>435</v>
+        <v>527</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" location="region"/>
-    <hyperlink ref="D8" r:id="rId2" location="region why do we need to distinguish between province and state?"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -3881,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3894,12 +3858,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3908,526 +3872,544 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C8" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>398</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C9" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>399</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C10" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>400</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C11" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>445</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>446</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>447</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>448</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="14" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="14" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>244</v>
+        <v>542</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>477</v>
+        <v>543</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="13" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>508</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>478</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>480</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>508</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>481</v>
+        <v>462</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>482</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>508</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>483</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>514</v>
+        <v>490</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>524</v>
+        <v>500</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>525</v>
+        <v>501</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>516</v>
+        <v>492</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>526</v>
+        <v>502</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>527</v>
+        <v>503</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>520</v>
+        <v>496</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>523</v>
+        <v>499</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>528</v>
+        <v>504</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>521</v>
+        <v>497</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>522</v>
+        <v>498</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>546</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>507</v>
+      </c>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="D46" s="5"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D47" s="5"/>
@@ -4489,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -4502,7 +4484,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -4513,27 +4495,27 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -4542,7 +4524,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -4554,78 +4536,75 @@
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="D8" t="s">
-        <v>497</v>
+        <v>523</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D11" t="s">
-        <v>496</v>
+        <v>544</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D12" t="s">
-        <v>498</v>
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4655,15 +4634,15 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>535</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>537</v>
+        <v>511</v>
       </c>
       <c r="C2" t="s">
-        <v>536</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -4674,99 +4653,99 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>539</v>
+        <v>513</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>541</v>
+        <v>515</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>542</v>
+        <v>516</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>538</v>
+        <v>512</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>543</v>
+        <v>517</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>544</v>
+        <v>518</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>545</v>
+        <v>519</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>546</v>
+        <v>520</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>547</v>
+        <v>521</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
edits to person onto
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-456" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-456" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="549">
   <si>
     <t>Requirement</t>
   </si>
@@ -745,9 +745,6 @@
     <t>Describing the department of a person</t>
   </si>
   <si>
-    <t>Person, hasDepartment, Department</t>
-  </si>
-  <si>
     <t>Describing the organizations a person is affiliated with</t>
   </si>
   <si>
@@ -1427,9 +1424,6 @@
   </si>
   <si>
     <t>foaf:homePage</t>
-  </si>
-  <si>
-    <t>why not isActive?</t>
   </si>
   <si>
     <t>should use foaf:mbox. If confusing we could use vcard:email or http://www.w3.org/2006/vcard/ns#hasEmail</t>
@@ -1695,6 +1689,15 @@
   </si>
   <si>
     <t>P43</t>
+  </si>
+  <si>
+    <t>Department, hasAffiliate, Person</t>
+  </si>
+  <si>
+    <t>SEE ADDRESS</t>
+  </si>
+  <si>
+    <t>why not isActive?hasStatus?</t>
   </si>
 </sst>
 </file>
@@ -2401,18 +2404,18 @@
         <v>8</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2426,7 +2429,7 @@
     </row>
     <row r="5" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -2437,7 +2440,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>23</v>
@@ -2448,7 +2451,7 @@
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -2459,7 +2462,7 @@
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -2470,7 +2473,7 @@
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>24</v>
@@ -2481,7 +2484,7 @@
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -2492,7 +2495,7 @@
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -2503,7 +2506,7 @@
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
@@ -2514,7 +2517,7 @@
     </row>
     <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>25</v>
@@ -2525,7 +2528,7 @@
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -2536,7 +2539,7 @@
     </row>
     <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>28</v>
@@ -2545,12 +2548,12 @@
         <v>29</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -2561,7 +2564,7 @@
     </row>
     <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>32</v>
@@ -2572,7 +2575,7 @@
     </row>
     <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>34</v>
@@ -2583,7 +2586,7 @@
     </row>
     <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -2594,7 +2597,7 @@
     </row>
     <row r="20" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>38</v>
@@ -2605,21 +2608,21 @@
     </row>
     <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>41</v>
@@ -2630,18 +2633,18 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>47</v>
@@ -2652,7 +2655,7 @@
     </row>
     <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>48</v>
@@ -2663,7 +2666,7 @@
     </row>
     <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>49</v>
@@ -2674,7 +2677,7 @@
     </row>
     <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>51</v>
@@ -2685,7 +2688,7 @@
     </row>
     <row r="28" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>53</v>
@@ -2694,12 +2697,12 @@
         <v>54</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>55</v>
@@ -2710,7 +2713,7 @@
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>57</v>
@@ -2721,7 +2724,7 @@
     </row>
     <row r="31" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>59</v>
@@ -2730,12 +2733,12 @@
         <v>3</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>60</v>
@@ -2746,7 +2749,7 @@
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>62</v>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
@@ -2768,7 +2771,7 @@
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>66</v>
@@ -2779,7 +2782,7 @@
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>68</v>
@@ -2790,7 +2793,7 @@
     </row>
     <row r="37" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>70</v>
@@ -2799,12 +2802,12 @@
         <v>71</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>72</v>
@@ -2813,12 +2816,12 @@
         <v>73</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>74</v>
@@ -2827,12 +2830,12 @@
         <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>76</v>
@@ -2841,12 +2844,12 @@
         <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>78</v>
@@ -2855,12 +2858,12 @@
         <v>168</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>79</v>
@@ -2869,12 +2872,12 @@
         <v>169</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>80</v>
@@ -2883,50 +2886,50 @@
         <v>170</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B47" t="s">
         <v>81</v>
@@ -2937,7 +2940,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B48" t="s">
         <v>82</v>
@@ -2948,7 +2951,7 @@
     </row>
     <row r="49" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>83</v>
@@ -2959,7 +2962,7 @@
     </row>
     <row r="50" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>84</v>
@@ -2970,7 +2973,7 @@
     </row>
     <row r="51" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>85</v>
@@ -2981,7 +2984,7 @@
     </row>
     <row r="52" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>86</v>
@@ -2992,7 +2995,7 @@
     </row>
     <row r="53" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>87</v>
@@ -3003,7 +3006,7 @@
     </row>
     <row r="54" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>88</v>
@@ -3014,7 +3017,7 @@
     </row>
     <row r="55" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>89</v>
@@ -3025,7 +3028,7 @@
     </row>
     <row r="56" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>90</v>
@@ -3036,7 +3039,7 @@
     </row>
     <row r="57" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>91</v>
@@ -3047,7 +3050,7 @@
     </row>
     <row r="58" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>92</v>
@@ -3058,7 +3061,7 @@
     </row>
     <row r="59" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>93</v>
@@ -3069,7 +3072,7 @@
     </row>
     <row r="60" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>94</v>
@@ -3080,7 +3083,7 @@
     </row>
     <row r="61" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>95</v>
@@ -3091,7 +3094,7 @@
     </row>
     <row r="62" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>96</v>
@@ -3102,7 +3105,7 @@
     </row>
     <row r="63" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>97</v>
@@ -3113,7 +3116,7 @@
     </row>
     <row r="64" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>98</v>
@@ -3124,7 +3127,7 @@
     </row>
     <row r="65" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>99</v>
@@ -3135,7 +3138,7 @@
     </row>
     <row r="66" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>100</v>
@@ -3146,7 +3149,7 @@
     </row>
     <row r="67" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>101</v>
@@ -3157,7 +3160,7 @@
     </row>
     <row r="68" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>102</v>
@@ -3168,7 +3171,7 @@
     </row>
     <row r="69" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>103</v>
@@ -3179,7 +3182,7 @@
     </row>
     <row r="70" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>104</v>
@@ -3190,7 +3193,7 @@
     </row>
     <row r="71" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>105</v>
@@ -3201,7 +3204,7 @@
     </row>
     <row r="72" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>106</v>
@@ -3212,7 +3215,7 @@
     </row>
     <row r="73" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>107</v>
@@ -3223,7 +3226,7 @@
     </row>
     <row r="74" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>108</v>
@@ -3234,7 +3237,7 @@
     </row>
     <row r="75" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>109</v>
@@ -3245,7 +3248,7 @@
     </row>
     <row r="76" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>110</v>
@@ -3256,7 +3259,7 @@
     </row>
     <row r="77" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>111</v>
@@ -3267,7 +3270,7 @@
     </row>
     <row r="78" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>112</v>
@@ -3278,7 +3281,7 @@
     </row>
     <row r="79" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>113</v>
@@ -3289,7 +3292,7 @@
     </row>
     <row r="80" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>114</v>
@@ -3300,7 +3303,7 @@
     </row>
     <row r="81" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>115</v>
@@ -3311,7 +3314,7 @@
     </row>
     <row r="82" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>116</v>
@@ -3322,7 +3325,7 @@
     </row>
     <row r="83" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B83" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -3357,7 +3360,7 @@
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3371,7 +3374,7 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3382,7 +3385,7 @@
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>118</v>
@@ -3393,7 +3396,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>120</v>
@@ -3404,7 +3407,7 @@
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>122</v>
@@ -3415,7 +3418,7 @@
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>124</v>
@@ -3426,7 +3429,7 @@
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>126</v>
@@ -3437,7 +3440,7 @@
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>128</v>
@@ -3448,7 +3451,7 @@
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>130</v>
@@ -3459,7 +3462,7 @@
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>132</v>
@@ -3470,7 +3473,7 @@
     </row>
     <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>134</v>
@@ -3481,7 +3484,7 @@
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>136</v>
@@ -3492,7 +3495,7 @@
     </row>
     <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>138</v>
@@ -3503,7 +3506,7 @@
     </row>
     <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>140</v>
@@ -3514,7 +3517,7 @@
     </row>
     <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>142</v>
@@ -3525,7 +3528,7 @@
     </row>
     <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>144</v>
@@ -3536,7 +3539,7 @@
     </row>
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>147</v>
@@ -3547,7 +3550,7 @@
     </row>
     <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>148</v>
@@ -3558,7 +3561,7 @@
     </row>
     <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>150</v>
@@ -3569,7 +3572,7 @@
     </row>
     <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>152</v>
@@ -3580,7 +3583,7 @@
     </row>
     <row r="23" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>154</v>
@@ -3591,7 +3594,7 @@
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>156</v>
@@ -3602,7 +3605,7 @@
     </row>
     <row r="25" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>158</v>
@@ -3613,7 +3616,7 @@
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>159</v>
@@ -3624,7 +3627,7 @@
     </row>
     <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>161</v>
@@ -3635,7 +3638,7 @@
     </row>
     <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>163</v>
@@ -3659,8 +3662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3674,12 +3677,12 @@
         <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3693,7 +3696,7 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>206</v>
@@ -3704,118 +3707,118 @@
     </row>
     <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>208</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>209</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>210</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>211</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>212</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>213</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>214</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B12" t="s">
         <v>215</v>
       </c>
       <c r="C12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -3833,8 +3836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3851,7 +3854,7 @@
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3865,7 +3868,7 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>218</v>
@@ -3874,12 +3877,12 @@
         <v>219</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>220</v>
@@ -3888,12 +3891,12 @@
         <v>221</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>222</v>
@@ -3902,12 +3905,12 @@
         <v>223</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>228</v>
@@ -3918,7 +3921,7 @@
     </row>
     <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>225</v>
@@ -3929,7 +3932,7 @@
     </row>
     <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>226</v>
@@ -3940,7 +3943,7 @@
     </row>
     <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>227</v>
@@ -3951,7 +3954,7 @@
     </row>
     <row r="11" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>229</v>
@@ -3962,7 +3965,7 @@
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>233</v>
@@ -3974,429 +3977,427 @@
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>236</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="13" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="B14" s="13" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="11" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>484</v>
-      </c>
+      <c r="C14" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="D14"/>
     </row>
     <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>240</v>
-      </c>
       <c r="D16" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>247</v>
-      </c>
       <c r="D19" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>249</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="B22" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="B22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>484</v>
+      <c r="D22" s="12" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>256</v>
-      </c>
       <c r="D23" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>261</v>
-      </c>
       <c r="D26" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>263</v>
-      </c>
       <c r="D27" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B28" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>265</v>
-      </c>
       <c r="D28" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="D29" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>271</v>
       </c>
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>273</v>
-      </c>
       <c r="D32" s="12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>277</v>
-      </c>
       <c r="D34" s="9" t="s">
-        <v>466</v>
+        <v>548</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>486</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>490</v>
-      </c>
       <c r="C37" s="5" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>489</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>491</v>
       </c>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4472,7 +4473,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -4488,22 +4489,22 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -4512,7 +4513,7 @@
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -4524,75 +4525,75 @@
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>292</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>293</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>300</v>
-      </c>
       <c r="D11" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>302</v>
-      </c>
       <c r="D12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -4622,15 +4623,15 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -4646,94 +4647,94 @@
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>510</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>514</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated person ontology affiliation model and added foaf props
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\EnigmaOntology\requirements\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-456" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="544">
   <si>
     <t>Requirement</t>
   </si>
@@ -748,9 +743,6 @@
     <t>Describing the organizations a person is affiliated with</t>
   </si>
   <si>
-    <t>Person, isAffiliatedWith, Organization</t>
-  </si>
-  <si>
     <t>Person, hasPublication, ENIGMAPublication</t>
   </si>
   <si>
@@ -790,36 +782,21 @@
     <t>Describing the location of a person</t>
   </si>
   <si>
-    <t>Person, isLocated, Location</t>
-  </si>
-  <si>
     <t>Describing the working groups a person is a member of</t>
   </si>
   <si>
-    <t>Person, isMemberOfWG, WorkingGroup</t>
-  </si>
-  <si>
     <t>Describing the working groups a person is a chair of</t>
   </si>
   <si>
-    <t>Person, isChairOfWG, WorkingGroup</t>
-  </si>
-  <si>
     <t>Describing the organizations a person was affiliated with</t>
   </si>
   <si>
     <t>Describing the email of person</t>
   </si>
   <si>
-    <t>Person, hasEmail, [string]</t>
-  </si>
-  <si>
     <t>Describing the first name of a person</t>
   </si>
   <si>
-    <t>Person, hasFirstName, [string]</t>
-  </si>
-  <si>
     <t>Describing the future publication instructions for a person</t>
   </si>
   <si>
@@ -829,9 +806,6 @@
     <t>Describing the last name of a person</t>
   </si>
   <si>
-    <t>Person, hasLastName, [string]</t>
-  </si>
-  <si>
     <t>Describing the middle initial of a person</t>
   </si>
   <si>
@@ -850,30 +824,9 @@
     <t>Person, hasTitle, {"Assistant professor" , "Associate professor" , "Graduate student" , "Other" , "Postdoctoral researcher" , "Professor" , "Program director" , "Program manager" , "Research assistant" , "Undergraduate"}</t>
   </si>
   <si>
-    <t>Person, hasWebsite, [string]</t>
-  </si>
-  <si>
     <t>Describing the webite of a person</t>
   </si>
   <si>
-    <t>Describing if a person is no longer active in ENIGMA</t>
-  </si>
-  <si>
-    <t>Person, isNoLongerActive, [boolean]</t>
-  </si>
-  <si>
-    <t>Describing the year a person first joined ENIGMA</t>
-  </si>
-  <si>
-    <t>Person, joinedEnigmaInYear, [year]</t>
-  </si>
-  <si>
-    <t>Describing the date a person left ENIGMA</t>
-  </si>
-  <si>
-    <t>Person, leftOnDate, [date]</t>
-  </si>
-  <si>
     <t>Describing if a cohort group includes people who are comorbid</t>
   </si>
   <si>
@@ -1397,36 +1350,6 @@
   </si>
   <si>
     <t>Should the range be a [string] instead of set? Depends on whether we accept more on "other"</t>
-  </si>
-  <si>
-    <t>Person should be foaf:Person</t>
-  </si>
-  <si>
-    <t>Why not project hasDataAnalyst Person??</t>
-  </si>
-  <si>
-    <t>Why do we need EnigmaPublication, not just "Publication"?</t>
-  </si>
-  <si>
-    <t>Redundant with Organization ontology</t>
-  </si>
-  <si>
-    <t>Why do we use abbreviation here? Not consistent</t>
-  </si>
-  <si>
-    <t>Same with abbreviation</t>
-  </si>
-  <si>
-    <t>should use foaf:givenName</t>
-  </si>
-  <si>
-    <t>should usefoaf:familyName</t>
-  </si>
-  <si>
-    <t>foaf:homePage</t>
-  </si>
-  <si>
-    <t>should use foaf:mbox. If confusing we could use vcard:email or http://www.w3.org/2006/vcard/ns#hasEmail</t>
   </si>
   <si>
     <t>WG1</t>
@@ -1664,15 +1587,9 @@
     <t>Organization, hasPrimaryAddress, Address</t>
   </si>
   <si>
-    <t>Separate to a separate module called ENIGMA roles</t>
-  </si>
-  <si>
     <t>Person, hasDegree, string</t>
   </si>
   <si>
-    <t>Change to string</t>
-  </si>
-  <si>
     <t>Clarify in the definition</t>
   </si>
   <si>
@@ -1694,17 +1611,80 @@
     <t>Department, hasAffiliate, Person</t>
   </si>
   <si>
-    <t>SEE ADDRESS</t>
-  </si>
-  <si>
-    <t>why not isActive?hasStatus?</t>
+    <t>WorkingGroup, hasWorkingGroupMember, Person</t>
+  </si>
+  <si>
+    <t>WorkingGroup, hasWorkingGroupChair, Person</t>
+  </si>
+  <si>
+    <t>Person, foaf:mbox, owl:Thing</t>
+  </si>
+  <si>
+    <t>Person, foaf:givenName, [string]</t>
+  </si>
+  <si>
+    <t>Person, foaf:familyName, [string]</t>
+  </si>
+  <si>
+    <t>Person, foaf:homePage, ???</t>
+  </si>
+  <si>
+    <t>what should the range be? Foaf uses foaf:document</t>
+  </si>
+  <si>
+    <t>QualifiedAffiliationRelationship, hasStatus, {"Active" , "Inactive" , "Left Organization"}</t>
+  </si>
+  <si>
+    <t>Describing the start date of a person in an organization</t>
+  </si>
+  <si>
+    <t>Describing the end date of a person in an organization</t>
+  </si>
+  <si>
+    <t>QualifiedAffiliationRelationship, hasStartDate, [date]</t>
+  </si>
+  <si>
+    <t>QualifiedAffiliationRelationship, hasEndDate [date]</t>
+  </si>
+  <si>
+    <t>Describing the activity status of a person in an organization</t>
+  </si>
+  <si>
+    <t>P44</t>
+  </si>
+  <si>
+    <t>Describing the detailed affiliation relationship of a person</t>
+  </si>
+  <si>
+    <t>Person, hasQualifiedAffiliationRelationship, QualifiedAffiliationRelationship</t>
+  </si>
+  <si>
+    <t>See P33 and P34</t>
+  </si>
+  <si>
+    <t>See P31 and P13</t>
+  </si>
+  <si>
+    <t>Person, vivo:orchidId, ???</t>
+  </si>
+  <si>
+    <t>what should the range be?</t>
+  </si>
+  <si>
+    <t>P45</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, Address</t>
+  </si>
+  <si>
+    <t>What is the primary address of an person?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1778,13 +1758,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -1819,6 +1792,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1848,7 +1833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1874,23 +1859,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="66">
+  <cellStyleXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1950,15 +1920,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1976,14 +1964,13 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="60"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="59"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="61"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="62"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="59" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="60"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="59"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="61"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="60" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="62" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="66">
+  <cellStyles count="84">
     <cellStyle name="Accent2" xfId="62" builtinId="33"/>
     <cellStyle name="Bad" xfId="60" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2017,6 +2004,15 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="59" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2047,6 +2043,15 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="61" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -2388,34 +2393,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.796875" customWidth="1"/>
+    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C1" s="10" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22.75">
       <c r="B2" s="2"/>
-      <c r="C2" s="11" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>302</v>
+      <c r="C2" s="10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" thickBot="1">
+      <c r="A4" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2427,9 +2432,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="17" thickTop="1">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -2438,9 +2443,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="17.5">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>23</v>
@@ -2449,9 +2454,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="17.5">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -2460,9 +2465,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -2471,9 +2476,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="17.5">
       <c r="A9" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>24</v>
@@ -2482,9 +2487,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="17.5">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -2493,9 +2498,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="17.5">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -2504,9 +2509,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="17.5">
       <c r="A12" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
@@ -2515,9 +2520,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="17.5">
       <c r="A13" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>25</v>
@@ -2526,9 +2531,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="17.5">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
@@ -2537,45 +2542,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:4" s="9" customFormat="1">
+      <c r="A15" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="D15" s="9" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="9" customFormat="1">
+      <c r="A16" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="1:4" s="9" customFormat="1">
+      <c r="A17" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="17.5">
       <c r="A18" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>34</v>
@@ -2584,9 +2589,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="17.5">
       <c r="A19" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>36</v>
@@ -2595,9 +2600,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="17.5">
       <c r="A20" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>38</v>
@@ -2606,23 +2611,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="B21" s="11" t="s">
+    <row r="21" spans="1:4" s="10" customFormat="1">
+      <c r="A21" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="C21" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.5">
       <c r="A22" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>41</v>
@@ -2631,20 +2636,20 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17.5">
       <c r="A24" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>47</v>
@@ -2653,9 +2658,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="17.5">
       <c r="A25" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>48</v>
@@ -2664,9 +2669,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="17.5">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>49</v>
@@ -2675,9 +2680,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="17.5">
       <c r="A27" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>51</v>
@@ -2686,23 +2691,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="B28" s="12" t="s">
+    <row r="28" spans="1:4" s="11" customFormat="1">
+      <c r="A28" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="D28" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17.5">
       <c r="A29" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>55</v>
@@ -2711,9 +2716,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="17.5">
       <c r="A30" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>57</v>
@@ -2722,23 +2727,23 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="B31" s="12" t="s">
+    <row r="31" spans="1:4" s="11" customFormat="1">
+      <c r="A31" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="D31" s="11" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17.5">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>60</v>
@@ -2747,9 +2752,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="17.5">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>62</v>
@@ -2758,9 +2763,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
@@ -2769,9 +2774,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="17.5">
       <c r="A35" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>66</v>
@@ -2780,9 +2785,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="17.5">
       <c r="A36" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>68</v>
@@ -2791,37 +2796,37 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="B37" s="12" t="s">
+    <row r="37" spans="1:4" s="11" customFormat="1">
+      <c r="A37" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="B38" s="12" t="s">
+      <c r="D37" s="11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="11" customFormat="1">
+      <c r="A38" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="D38" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17.5">
       <c r="A39" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>74</v>
@@ -2830,12 +2835,12 @@
         <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17.5">
       <c r="A40" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>76</v>
@@ -2844,92 +2849,92 @@
         <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="B41" s="10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="9" customFormat="1">
+      <c r="A41" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="B42" s="10" t="s">
+      <c r="D41" s="9" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="9" customFormat="1">
+      <c r="A42" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="B43" s="10" t="s">
+      <c r="D42" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="9" customFormat="1">
+      <c r="A43" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="D43" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17.5">
       <c r="A44" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17.5">
       <c r="A45" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="17.5">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="B47" t="s">
         <v>81</v>
@@ -2938,9 +2943,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="B48" t="s">
         <v>82</v>
@@ -2949,9 +2954,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="17.5">
       <c r="A49" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>83</v>
@@ -2960,9 +2965,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="17.5">
       <c r="A50" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>84</v>
@@ -2971,9 +2976,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="17.5">
       <c r="A51" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>85</v>
@@ -2982,9 +2987,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="17.5">
       <c r="A52" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>86</v>
@@ -2993,9 +2998,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="17.5">
       <c r="A53" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>87</v>
@@ -3004,9 +3009,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="17.5">
       <c r="A54" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>88</v>
@@ -3015,9 +3020,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="17.5">
       <c r="A55" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>89</v>
@@ -3026,9 +3031,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="17.5">
       <c r="A56" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>90</v>
@@ -3037,9 +3042,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="17.5">
       <c r="A57" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>91</v>
@@ -3048,9 +3053,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="17.5">
       <c r="A58" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>92</v>
@@ -3059,9 +3064,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="17.5">
       <c r="A59" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>93</v>
@@ -3070,9 +3075,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="17.5">
       <c r="A60" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>94</v>
@@ -3081,9 +3086,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="17.5">
       <c r="A61" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>95</v>
@@ -3092,9 +3097,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="17.5">
       <c r="A62" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>96</v>
@@ -3103,9 +3108,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="17.5">
       <c r="A63" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>97</v>
@@ -3114,9 +3119,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="17.5">
       <c r="A64" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>98</v>
@@ -3125,9 +3130,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="17.5">
       <c r="A65" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>99</v>
@@ -3136,9 +3141,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" ht="17.5">
       <c r="A66" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>100</v>
@@ -3147,9 +3152,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="17.5">
       <c r="A67" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>101</v>
@@ -3158,9 +3163,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="17.5">
       <c r="A68" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>102</v>
@@ -3169,9 +3174,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="17.5">
       <c r="A69" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>103</v>
@@ -3180,9 +3185,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="17.5">
       <c r="A70" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>104</v>
@@ -3191,9 +3196,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="17.5">
       <c r="A71" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>105</v>
@@ -3202,9 +3207,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" ht="17.5">
       <c r="A72" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>106</v>
@@ -3213,9 +3218,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="17.5">
       <c r="A73" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>107</v>
@@ -3224,9 +3229,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="17.5">
       <c r="A74" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>108</v>
@@ -3235,9 +3240,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="17.5">
       <c r="A75" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>109</v>
@@ -3246,9 +3251,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="17.5">
       <c r="A76" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>110</v>
@@ -3257,9 +3262,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" ht="17.5">
       <c r="A77" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>111</v>
@@ -3268,9 +3273,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="17.5">
       <c r="A78" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>112</v>
@@ -3279,9 +3284,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" ht="17.5">
       <c r="A79" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>113</v>
@@ -3290,9 +3295,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" ht="17.5">
       <c r="A80" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>114</v>
@@ -3301,9 +3306,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" ht="17.5">
       <c r="A81" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>115</v>
@@ -3312,9 +3317,9 @@
         <v>203</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" ht="17.5">
       <c r="A82" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>116</v>
@@ -3323,9 +3328,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" ht="17.5">
       <c r="B83" s="5" t="s">
-        <v>520</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -3344,23 +3349,23 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>302</v>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3372,9 +3377,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3383,9 +3388,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="17.5">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>118</v>
@@ -3394,9 +3399,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="17.5">
       <c r="A6" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>120</v>
@@ -3405,9 +3410,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="17.5">
       <c r="A7" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>122</v>
@@ -3416,9 +3421,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5">
       <c r="A8" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>124</v>
@@ -3427,9 +3432,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="17.5">
       <c r="A9" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>126</v>
@@ -3438,9 +3443,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="17.5">
       <c r="A10" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>128</v>
@@ -3449,9 +3454,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="17.5">
       <c r="A11" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>130</v>
@@ -3460,9 +3465,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="17.5">
       <c r="A12" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>132</v>
@@ -3471,9 +3476,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="17.5">
       <c r="A13" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>134</v>
@@ -3482,9 +3487,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="17.5">
       <c r="A14" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>136</v>
@@ -3493,9 +3498,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="17.5">
       <c r="A15" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>138</v>
@@ -3504,9 +3509,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="17.5">
       <c r="A16" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>140</v>
@@ -3515,9 +3520,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="17.5">
       <c r="A17" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>142</v>
@@ -3526,9 +3531,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="17.5">
       <c r="A18" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>144</v>
@@ -3537,9 +3542,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="17.5">
       <c r="A19" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>147</v>
@@ -3548,9 +3553,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="17.5">
       <c r="A20" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>148</v>
@@ -3559,9 +3564,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="17.5">
       <c r="A21" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>150</v>
@@ -3570,9 +3575,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="17.5">
       <c r="A22" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>152</v>
@@ -3581,9 +3586,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="17.5">
       <c r="A23" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>154</v>
@@ -3592,9 +3597,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="17.5">
       <c r="A24" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>156</v>
@@ -3603,9 +3608,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="17.5">
       <c r="A25" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>158</v>
@@ -3614,9 +3619,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="17.5">
       <c r="A26" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>159</v>
@@ -3625,9 +3630,9 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="17.5">
       <c r="A27" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>161</v>
@@ -3636,9 +3641,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="17.5">
       <c r="A28" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>163</v>
@@ -3662,27 +3667,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>302</v>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>288</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3694,9 +3699,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>417</v>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+      <c r="A4" s="5" t="s">
+        <v>403</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>206</v>
@@ -3705,120 +3710,120 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A5" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>526</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="C5" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A6" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="C6" s="5" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A7" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="C7" s="5" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>529</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C8" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A9" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="C9" s="5" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A10" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="C10" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A11" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>425</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C11" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C12" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>503</v>
-      </c>
-      <c r="B13" t="s">
-        <v>504</v>
-      </c>
-      <c r="C13" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>525</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>536</v>
+      <c r="C12" s="5" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A13" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>482</v>
+      </c>
+      <c r="B14" t="s">
+        <v>501</v>
+      </c>
+      <c r="C14" t="s">
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -3834,27 +3839,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="76.296875" customWidth="1"/>
-    <col min="3" max="3" width="90.796875" customWidth="1"/>
-    <col min="4" max="4" width="26.69921875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" customWidth="1"/>
+    <col min="3" max="3" width="90.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>302</v>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="A3" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3866,9 +3872,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>387</v>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+      <c r="A4" s="5" t="s">
+        <v>373</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>218</v>
@@ -3876,96 +3882,87 @@
       <c r="C4" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="B5" s="12" t="s">
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A5" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>389</v>
-      </c>
-      <c r="B6" s="12" t="s">
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A6" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>390</v>
-      </c>
-      <c r="B7" s="12" t="s">
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A7" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A9" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A10" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>429</v>
-      </c>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A11" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>430</v>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>416</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>233</v>
@@ -3973,477 +3970,459 @@
       <c r="C12" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" s="14" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>431</v>
-      </c>
-      <c r="B13" s="14" t="s">
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A13" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>538</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="11" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="C13" s="5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A14" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>237</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>546</v>
-      </c>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>433</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A15" s="5" t="s">
+        <v>419</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>434</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A16" s="5" t="s">
+        <v>420</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A17" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A18" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A19" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A20" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A21" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A22" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A23" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A24" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A25" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A26" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A27" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="13" customFormat="1" ht="16">
+      <c r="A28" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A29" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A30" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A31" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B31" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A32" s="12" t="s">
         <v>436</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B32" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A33" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="B33" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A34" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="B34" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A35" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="B35" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A36" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>441</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="B36" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A37" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A38" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>442</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>443</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>444</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D26" s="9" t="s">
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A39" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>445</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>446</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>447</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>448</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>449</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>451</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>452</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>453</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>454</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>486</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="D37" s="5"/>
-    </row>
-    <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A40" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A41" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A42" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A43" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A44" s="12" t="s">
+        <v>517</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A45" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A46" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="C46" s="5" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A47" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>501</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>502</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="C47" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A48" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>545</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="4:4" ht="16">
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" ht="17.5">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" ht="17.5">
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" ht="17.5">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" ht="17.5">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" ht="17.5">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="55" spans="4:4" ht="17.5">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="56" spans="4:4" ht="17.5">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="57" spans="4:4" ht="17.5">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="58" spans="4:4" ht="17.5">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="59" spans="4:4" ht="17.5">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="60" spans="4:4" ht="17.5">
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="4:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="61" spans="4:4" ht="17.5">
       <c r="D61" s="5"/>
+    </row>
+    <row r="62" spans="4:4" ht="17.5">
+      <c r="D62" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4461,22 +4440,25 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>288</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4487,33 +4469,33 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="17.5">
       <c r="A5" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="17.5">
       <c r="A6" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -4523,77 +4505,77 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="17.5">
       <c r="A7" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5">
       <c r="A8" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17.5">
       <c r="A9" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17.5">
       <c r="A10" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17.5">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="D11" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.5">
       <c r="A12" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="D12" t="s">
-        <v>541</v>
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -4611,30 +4593,33 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>288</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4645,103 +4630,108 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="17.5">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="17.5">
       <c r="A6" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>514</v>
+        <v>490</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="17.5">
       <c r="A7" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5">
       <c r="A8" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>516</v>
+        <v>492</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17.5">
       <c r="A9" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17.5">
       <c r="A10" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17.5">
       <c r="A11" t="s">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.5">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more requirement editing. Deleted a few roles
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\EnigmaOntology\requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -13,6 +18,7 @@
     <sheet name="Person Ontology" sheetId="5" r:id="rId4"/>
     <sheet name="WorkingGroup Ontology" sheetId="6" r:id="rId5"/>
     <sheet name="Protocol Ontology" sheetId="8" r:id="rId6"/>
+    <sheet name="Role Ontology" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="594">
   <si>
     <t>Requirement</t>
   </si>
@@ -758,18 +764,9 @@
     <t>Describing the cohorts a person is a principal investigator of</t>
   </si>
   <si>
-    <t>Person, isPIOf, Cohort</t>
-  </si>
-  <si>
     <t>Describing the cohorts a person is a main principal investigator of</t>
   </si>
   <si>
-    <t>Person, isMainPIOf, Cohort</t>
-  </si>
-  <si>
-    <t>Is this requirement still necessary?</t>
-  </si>
-  <si>
     <t>Describing the cohorts a person is  a minor principal investigator of</t>
   </si>
   <si>
@@ -1373,18 +1370,12 @@
     <t>CLARIFY IF HAS IS THE SAME AS INCLUDES</t>
   </si>
   <si>
-    <t>REMOVED</t>
-  </si>
-  <si>
     <t>Person, isContactOf, Cohort</t>
   </si>
   <si>
     <t>Person, hasAddress, Address</t>
   </si>
   <si>
-    <t>p34</t>
-  </si>
-  <si>
     <t>Describing the street address of a person</t>
   </si>
   <si>
@@ -1418,21 +1409,6 @@
     <t>Address, country name, [string]</t>
   </si>
   <si>
-    <t>p35</t>
-  </si>
-  <si>
-    <t>p36</t>
-  </si>
-  <si>
-    <t>p37</t>
-  </si>
-  <si>
-    <t>p38</t>
-  </si>
-  <si>
-    <t>p39</t>
-  </si>
-  <si>
     <t>O10</t>
   </si>
   <si>
@@ -1490,9 +1466,6 @@
     <t>Describing the Memorandum of understanding of a working group</t>
   </si>
   <si>
-    <t>What is the role of a person in an organization?</t>
-  </si>
-  <si>
     <t>What organizations did a person belong to?</t>
   </si>
   <si>
@@ -1568,9 +1541,6 @@
     <t>Person, foaf:familyName, [string]</t>
   </si>
   <si>
-    <t>Person, foaf:homePage, ???</t>
-  </si>
-  <si>
     <t>QualifiedAffiliationRelationship, hasStatus, {"Active" , "Inactive" , "Left Organization"}</t>
   </si>
   <si>
@@ -1604,9 +1574,6 @@
     <t>See P31 and P13</t>
   </si>
   <si>
-    <t>Person, vivo:orchidId, ???</t>
-  </si>
-  <si>
     <t>P45</t>
   </si>
   <si>
@@ -1622,19 +1589,10 @@
     <t>WorkingGroup, hasMemorandumOfUnderstanding, [string]</t>
   </si>
   <si>
-    <t>should this be QualifiedAffiliation or person</t>
-  </si>
-  <si>
     <t>WG10</t>
   </si>
   <si>
-    <t>Describing the abbreviated name</t>
-  </si>
-  <si>
     <t>WG11</t>
-  </si>
-  <si>
-    <t>Describing the full name</t>
   </si>
   <si>
     <t>WG12</t>
@@ -1676,9 +1634,6 @@
     <t>P46</t>
   </si>
   <si>
-    <t>What is the grant is associated with the person?</t>
-  </si>
-  <si>
     <t>Secondary Proposal Form</t>
   </si>
   <si>
@@ -1691,17 +1646,200 @@
     <t>TODO (should be own class)</t>
   </si>
   <si>
-    <t>as string for each person</t>
-  </si>
-  <si>
     <t>Pr26</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Who contributed to writing a paper?</t>
+  </si>
+  <si>
+    <t>Who contributed to the design of a project?</t>
+  </si>
+  <si>
+    <t>Who wrote the first draft of a paper?</t>
+  </si>
+  <si>
+    <t>Who read the paper?</t>
+  </si>
+  <si>
+    <t>Should have as domain a project/Paper and range person</t>
+  </si>
+  <si>
+    <t>Which author has a conflict in a publication?</t>
+  </si>
+  <si>
+    <t>If an author has a conflict with a publication, which is it?</t>
+  </si>
+  <si>
+    <t>What is the abbreviated name of a working group? It's difficult to call them by their complete names because it's too long</t>
+  </si>
+  <si>
+    <t>What is the full name of a WG?</t>
+  </si>
+  <si>
+    <t>What are the grants associated with a person?</t>
+  </si>
+  <si>
+    <t>Since projects have associated publications, we include the requirements for publications here too.</t>
+  </si>
+  <si>
+    <t>string could be a link to the memorandum</t>
+  </si>
+  <si>
+    <t>This should be addressed through the projects.</t>
+  </si>
+  <si>
+    <t>This is a secondary proposal form that is issued to do new projects based in a working group. Is it domain project or WG??</t>
+  </si>
+  <si>
+    <t>What is the status of the publication? (submitted, accepted, rejected, etc.)</t>
+  </si>
+  <si>
+    <t>What is the title of a publication</t>
+  </si>
+  <si>
+    <t>Who is an author of a publication?</t>
+  </si>
+  <si>
+    <t>Which conference was the publication sent to?</t>
+  </si>
+  <si>
+    <t>What is the link to the paper?</t>
+  </si>
+  <si>
+    <t>Which year was the paper written?</t>
+  </si>
+  <si>
+    <t>Which location was the publication presented in?</t>
+  </si>
+  <si>
+    <t>What cohorts have samples of a process?</t>
+  </si>
+  <si>
+    <t>Which cohorts have data files that are result from a given protocol?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO DO </t>
+  </si>
+  <si>
+    <t>Person, vivo:orchidId URI (range is a resource)</t>
+  </si>
+  <si>
+    <t>Person, foaf:homePage, URI (range is a resource)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMOVED: This feature is not finally required after agreement in meetings. </t>
+  </si>
+  <si>
+    <t>REMOVED: This was a misunderstanding, it wasn't a requirement</t>
+  </si>
+  <si>
+    <t>Should be dcterms:contributor</t>
+  </si>
+  <si>
+    <t>move to roles</t>
+  </si>
+  <si>
+    <t>What type of publication</t>
+  </si>
+  <si>
+    <t>Person, hasConflict, Conflict</t>
+  </si>
+  <si>
+    <t>Project, hasPublication, Publication</t>
+  </si>
+  <si>
+    <t>Conflict, dcterms:description, [string], inPublication, Publication</t>
+  </si>
+  <si>
+    <t>Should do an example to show how this works.</t>
+  </si>
+  <si>
+    <t>We don't reuse bibo because it adds a level of complexity</t>
+  </si>
+  <si>
+    <t>ENIGMAPublication is a bibo:AcademicArticle. Also may be bibo:Issue, bibo:Proceedings</t>
+  </si>
+  <si>
+    <t>ENIGMAPublication hasVenue, [string]</t>
+  </si>
+  <si>
+    <t>ENIGMAPublication dcterms:identifier, [string]</t>
+  </si>
+  <si>
+    <t>ENIGMAPublication  http://purl.org/dc/terms/date, [date]</t>
+  </si>
+  <si>
+    <t>ENIGMAPublication , http://purl.org/dc/terms/spatial, string</t>
+  </si>
+  <si>
+    <t>change to hasProjectBriefDescription</t>
+  </si>
+  <si>
+    <t>ENIGMAPublication, bibo:DocumentStatus (it has a limited set ofinstances)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ENIGMAPublication, http://purl.org/dc/terms/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ENIGMAPublication, http://purl.org/dc/terms/contributor</t>
+  </si>
+  <si>
+    <t>Person, isPrincipalInvestigatorOf, Cohort</t>
+  </si>
+  <si>
+    <t>Person, isMainPrincipalInvestigatorOf, Cohort</t>
+  </si>
+  <si>
+    <t>moved to roles</t>
+  </si>
+  <si>
+    <t>moved to roles. We only keep the most important ones in this ontology</t>
+  </si>
+  <si>
+    <t>What is the currento job title for a person?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person, currentJobTitle, string [examples: student, postdoc, faculty, staff]. </t>
+  </si>
+  <si>
+    <t>should add the 4 types in the definition</t>
+  </si>
+  <si>
+    <t>Person, hasGrant, string</t>
+  </si>
+  <si>
+    <t>Reason is that grants will be used in the acknowledgements</t>
+  </si>
+  <si>
+    <t>P34</t>
+  </si>
+  <si>
+    <t>P35</t>
+  </si>
+  <si>
+    <t>P36</t>
+  </si>
+  <si>
+    <t>P37</t>
+  </si>
+  <si>
+    <t>P38</t>
+  </si>
+  <si>
+    <t>P39</t>
+  </si>
+  <si>
+    <t>should be subprop of http://purl.org/dc/terms/contributor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1789,21 +1927,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -1826,8 +1951,38 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1847,11 +2002,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -1882,7 +2032,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1945,7 +2095,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1974,7 +2123,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1992,14 +2141,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="59"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="60" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="62" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="62"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="59" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="61" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="60" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="59" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="61" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="60"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="61"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="60" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="60" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="90">
-    <cellStyle name="Accent2" xfId="62" builtinId="33"/>
+  <cellStyles count="89">
     <cellStyle name="Bad" xfId="60" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2029,21 +2182,21 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="59" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2074,18 +2227,18 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="61" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -2425,36 +2578,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="90.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="22">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" thickBot="1">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2466,9 +2619,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
@@ -2477,9 +2630,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>22</v>
@@ -2488,9 +2641,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -2499,9 +2652,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
@@ -2510,9 +2663,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
@@ -2521,9 +2674,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
@@ -2532,9 +2685,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
@@ -2543,9 +2696,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
@@ -2554,9 +2707,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>24</v>
@@ -2565,9 +2718,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -2576,9 +2729,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>27</v>
@@ -2587,12 +2740,12 @@
         <v>28</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="16">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>29</v>
@@ -2601,9 +2754,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" ht="16">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>31</v>
@@ -2612,9 +2765,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>33</v>
@@ -2623,9 +2776,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>35</v>
@@ -2634,9 +2787,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>37</v>
@@ -2645,23 +2798,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="12" customFormat="1" ht="16">
-      <c r="A21" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="B21" s="12" t="s">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>540</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="C21" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>40</v>
@@ -2670,20 +2823,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>46</v>
@@ -2692,9 +2845,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>47</v>
@@ -2703,9 +2856,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>48</v>
@@ -2714,9 +2867,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
@@ -2725,23 +2878,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="13" customFormat="1" ht="16">
-      <c r="A28" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="B28" s="13" t="s">
+    <row r="28" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A28" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D28" s="11" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
@@ -2750,9 +2903,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>56</v>
@@ -2761,23 +2914,23 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="13" customFormat="1" ht="16">
-      <c r="A31" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B31" s="13" t="s">
+    <row r="31" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D31" s="11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>59</v>
@@ -2786,9 +2939,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>61</v>
@@ -2797,9 +2950,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>63</v>
@@ -2808,9 +2961,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>65</v>
@@ -2819,9 +2972,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>67</v>
@@ -2830,37 +2983,37 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="13" customFormat="1" ht="16">
-      <c r="A37" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B37" s="13" t="s">
+    <row r="37" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A37" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="13" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="13" customFormat="1" ht="16">
-      <c r="A38" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="B38" s="13" t="s">
+      <c r="D37" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D38" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>73</v>
@@ -2869,12 +3022,12 @@
         <v>74</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>75</v>
@@ -2883,12 +3036,12 @@
         <v>76</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="9" customFormat="1" ht="16">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>77</v>
@@ -2897,12 +3050,12 @@
         <v>167</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="9" customFormat="1" ht="16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>78</v>
@@ -2911,12 +3064,12 @@
         <v>168</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="9" customFormat="1" ht="16">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>79</v>
@@ -2925,50 +3078,50 @@
         <v>169</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
         <v>321</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A45" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A46" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A47" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>80</v>
@@ -2977,9 +3130,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>81</v>
@@ -2988,9 +3141,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="49" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>82</v>
@@ -2999,9 +3152,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="50" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>83</v>
@@ -3010,9 +3163,9 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="51" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>84</v>
@@ -3021,9 +3174,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="52" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>85</v>
@@ -3032,9 +3185,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="53" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>86</v>
@@ -3043,9 +3196,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="54" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>87</v>
@@ -3054,9 +3207,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="55" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>88</v>
@@ -3065,9 +3218,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="56" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>89</v>
@@ -3076,9 +3229,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="57" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>90</v>
@@ -3087,9 +3240,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="58" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>91</v>
@@ -3098,9 +3251,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="59" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>92</v>
@@ -3109,9 +3262,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="60" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>93</v>
@@ -3120,9 +3273,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>94</v>
@@ -3131,9 +3284,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="62" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>95</v>
@@ -3142,9 +3295,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="63" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>96</v>
@@ -3153,9 +3306,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>97</v>
@@ -3164,9 +3317,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>98</v>
@@ -3175,9 +3328,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="66" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>99</v>
@@ -3186,9 +3339,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="67" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>100</v>
@@ -3197,9 +3350,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="68" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>101</v>
@@ -3208,9 +3361,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="69" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>102</v>
@@ -3219,9 +3372,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="70" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>103</v>
@@ -3230,9 +3383,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="71" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>104</v>
@@ -3241,9 +3394,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="72" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>105</v>
@@ -3252,9 +3405,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="73" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>106</v>
@@ -3263,9 +3416,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>107</v>
@@ -3274,9 +3427,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="75" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>108</v>
@@ -3285,9 +3438,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="76" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>109</v>
@@ -3296,9 +3449,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>110</v>
@@ -3307,9 +3460,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="78" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>111</v>
@@ -3318,9 +3471,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="79" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>112</v>
@@ -3329,9 +3482,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="80" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>113</v>
@@ -3340,9 +3493,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="81" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>114</v>
@@ -3351,9 +3504,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="82" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>115</v>
@@ -3362,9 +3515,28 @@
         <v>203</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="83" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B83" s="5" t="s">
-        <v>486</v>
+        <v>476</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B84" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B85" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -3380,26 +3552,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+      <c r="C1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3411,9 +3586,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3422,20 +3597,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D5" s="17" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>119</v>
@@ -3444,86 +3622,107 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D7" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D8" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="12" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D9" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="12" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D10" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D11" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="12" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D12" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="12" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D13" s="17" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>135</v>
@@ -3532,9 +3731,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>137</v>
@@ -3543,9 +3742,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3554,9 +3753,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>141</v>
@@ -3565,9 +3764,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>143</v>
@@ -3576,9 +3775,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>146</v>
@@ -3587,9 +3786,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>147</v>
@@ -3598,9 +3797,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>149</v>
@@ -3609,9 +3808,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>151</v>
@@ -3619,10 +3818,13 @@
       <c r="C22" s="5" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D22" s="13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>153</v>
@@ -3631,20 +3833,23 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D24" s="17" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>157</v>
@@ -3653,9 +3858,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>158</v>
@@ -3664,9 +3869,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>160</v>
@@ -3675,9 +3880,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>162</v>
@@ -3686,15 +3891,104 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="9" customFormat="1" ht="16">
+    <row r="29" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B30" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B31" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="D31" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B32" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B33" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B34" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>547</v>
+      <c r="C34" s="16" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>570</v>
+      </c>
+      <c r="D35" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B36" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B37" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B38" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B39" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>569</v>
       </c>
     </row>
   </sheetData>
@@ -3713,26 +4007,26 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A4:XFD14"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>204</v>
       </c>
       <c r="C1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3744,9 +4038,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>205</v>
@@ -3755,120 +4049,120 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>207</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>208</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>209</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>210</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>211</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>212</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>213</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>491</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -3886,26 +4180,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.33203125" customWidth="1"/>
-    <col min="3" max="3" width="90.83203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.296875" customWidth="1"/>
+    <col min="3" max="3" width="90.796875" customWidth="1"/>
+    <col min="4" max="4" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3917,130 +4211,154 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="B5" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="15" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D5" s="5" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="15" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D6" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B7" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="15" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D7" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A9" s="5" t="s">
+      <c r="B11" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>405</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A11" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A12" s="5" t="s">
-        <v>408</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="12" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="D12" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>235</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>236</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>239</v>
@@ -4049,9 +4367,9 @@
         <v>238</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>237</v>
@@ -4060,20 +4378,20 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>240</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>241</v>
@@ -4082,392 +4400,397 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>243</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A20" s="9" t="s">
+      <c r="C20" s="5" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>414</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D21" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="11" customFormat="1">
-      <c r="A21" s="11" t="s">
+      <c r="B23" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="B24" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A22" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A23" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A24" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A25" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>253</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>421</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D28" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B29" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A27" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C27" s="5" t="s">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>587</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>590</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="10" customFormat="1" ht="16">
-      <c r="A28" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A29" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A30" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A31" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A32" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A33" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C33" s="5" t="s">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A34" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A35" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B48" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A36" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A37" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A38" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A39" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A40" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A41" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A42" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A43" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A44" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="C44" s="5" t="s">
+    <row r="49" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A49" s="9" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A45" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>488</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A46" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A47" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A48" s="5" t="s">
-        <v>527</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A49" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>542</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>543</v>
+      <c r="C49" s="9" t="s">
+        <v>585</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="16">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" ht="16">
+    <row r="51" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" ht="16">
+    <row r="52" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" ht="16">
+    <row r="53" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" ht="16">
+    <row r="54" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" ht="16">
+    <row r="55" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="16">
+    <row r="56" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="16">
+    <row r="57" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="16">
+    <row r="58" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="16">
+    <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="16">
+    <row r="60" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="D60" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4481,24 +4804,24 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4510,136 +4833,142 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A9" s="5" t="s">
+      <c r="B11" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B12" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A11" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A12" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A13" s="9" t="s">
-        <v>533</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>536</v>
-      </c>
       <c r="D13" s="9" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="9" customFormat="1" ht="16">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>535</v>
+        <v>520</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="13" customFormat="1" ht="16">
-      <c r="A15" s="13" t="s">
-        <v>537</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>545</v>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -4657,32 +4986,32 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A4:D11"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="C2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4694,103 +5023,103 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" thickTop="1">
+    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>483</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="5" t="s">
-        <v>376</v>
-      </c>
       <c r="B11" s="5" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="16">
+    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
@@ -4802,4 +5131,140 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>532</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed many things in the ontologies
Missing documentation and fixes in project
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Organization Ontology" sheetId="4" r:id="rId3"/>
     <sheet name="Person Ontology" sheetId="5" r:id="rId4"/>
     <sheet name="WorkingGroup Ontology" sheetId="6" r:id="rId5"/>
-    <sheet name="Protocol Ontology" sheetId="8" r:id="rId6"/>
-    <sheet name="Role Ontology" sheetId="10" r:id="rId7"/>
+    <sheet name="Role Ontology" sheetId="10" r:id="rId6"/>
+    <sheet name="Protocol Ontology" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="628">
   <si>
     <t>Requirement</t>
   </si>
@@ -386,15 +386,9 @@
     <t>Describing the contributors of a project</t>
   </si>
   <si>
-    <t>Project, hasContributor, Person</t>
-  </si>
-  <si>
     <t>Describing the contact person of a project</t>
   </si>
   <si>
-    <t>Project, hasContactPerson, Person</t>
-  </si>
-  <si>
     <t>Describing the data analysts of a project</t>
   </si>
   <si>
@@ -686,9 +680,6 @@
     <t>Describing the projects a person contributes to</t>
   </si>
   <si>
-    <t>Person, contributesTo, Project</t>
-  </si>
-  <si>
     <t>Describing the projects a person is a data analyst of</t>
   </si>
   <si>
@@ -731,9 +722,6 @@
     <t>Describing the projects a person is a project lead of</t>
   </si>
   <si>
-    <t>Person, isProjectLeadOf, Project</t>
-  </si>
-  <si>
     <t>Person, isProjectDeveloperOf, Project</t>
   </si>
   <si>
@@ -746,21 +734,12 @@
     <t>Describing the organizations a person is affiliated with</t>
   </si>
   <si>
-    <t>Person, hasPublication, ENIGMAPublication</t>
-  </si>
-  <si>
     <t>Describing the ENIGMA publications of a person</t>
   </si>
   <si>
-    <t>Describing the cohorts a person is an ENIGMA contact of</t>
-  </si>
-  <si>
     <t>Describing the cohorts a person is an investigator of</t>
   </si>
   <si>
-    <t>Person, isInvestigatorOf, Cohort</t>
-  </si>
-  <si>
     <t>Describing the cohorts a person is a principal investigator of</t>
   </si>
   <si>
@@ -809,15 +788,9 @@
     <t>Describing the research interests of person</t>
   </si>
   <si>
-    <t>Person, hasResearchInterests, [string]</t>
-  </si>
-  <si>
     <t>Describing the title of a person</t>
   </si>
   <si>
-    <t>Describing the webite of a person</t>
-  </si>
-  <si>
     <t>Describing if a cohort group includes people who are comorbid</t>
   </si>
   <si>
@@ -863,9 +836,6 @@
     <t>Describing the brief description of a working group</t>
   </si>
   <si>
-    <t>WorkingGroup, hasWGBriefDescription, [string]</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -1370,45 +1340,24 @@
     <t>CLARIFY IF HAS IS THE SAME AS INCLUDES</t>
   </si>
   <si>
-    <t>Person, isContactOf, Cohort</t>
-  </si>
-  <si>
-    <t>Person, hasAddress, Address</t>
-  </si>
-  <si>
     <t>Describing the street address of a person</t>
   </si>
   <si>
     <t>Describing the overall address of a person</t>
   </si>
   <si>
-    <t>Address, street address, [string]</t>
-  </si>
-  <si>
     <t>Describing the locality (city or town) of a person</t>
   </si>
   <si>
-    <t>Address, locality, [string]</t>
-  </si>
-  <si>
     <t>Describing the region (state or province) of a person</t>
   </si>
   <si>
-    <t>Address, region, [string]</t>
-  </si>
-  <si>
     <t>Describing the country of a person</t>
   </si>
   <si>
     <t>Describing the postal code of a person</t>
   </si>
   <si>
-    <t>Address, postal code, [string]</t>
-  </si>
-  <si>
-    <t>Address, country name, [string]</t>
-  </si>
-  <si>
     <t>O10</t>
   </si>
   <si>
@@ -1523,39 +1472,24 @@
     <t>P43</t>
   </si>
   <si>
-    <t>Department, hasAffiliate, Person</t>
-  </si>
-  <si>
     <t>WorkingGroup, hasWorkingGroupMember, Person</t>
   </si>
   <si>
     <t>WorkingGroup, hasWorkingGroupChair, Person</t>
   </si>
   <si>
-    <t>Person, foaf:mbox, owl:Thing</t>
-  </si>
-  <si>
     <t>Person, foaf:givenName, [string]</t>
   </si>
   <si>
     <t>Person, foaf:familyName, [string]</t>
   </si>
   <si>
-    <t>QualifiedAffiliationRelationship, hasStatus, {"Active" , "Inactive" , "Left Organization"}</t>
-  </si>
-  <si>
     <t>Describing the start date of a person in an organization</t>
   </si>
   <si>
     <t>Describing the end date of a person in an organization</t>
   </si>
   <si>
-    <t>QualifiedAffiliationRelationship, hasStartDate, [date]</t>
-  </si>
-  <si>
-    <t>QualifiedAffiliationRelationship, hasEndDate [date]</t>
-  </si>
-  <si>
     <t>Describing the activity status of a person in an organization</t>
   </si>
   <si>
@@ -1596,9 +1530,6 @@
   </si>
   <si>
     <t>WG12</t>
-  </si>
-  <si>
-    <t>TODO</t>
   </si>
   <si>
     <t>Describing the working group type (Healthy Variation, Genetic Studies, Methodology, and Clinical Populations)</t>
@@ -1628,9 +1559,6 @@
     </r>
   </si>
   <si>
-    <t>WorkingGroup, hasPublishedPaper, [string]</t>
-  </si>
-  <si>
     <t>P46</t>
   </si>
   <si>
@@ -1688,9 +1616,6 @@
     <t>string could be a link to the memorandum</t>
   </si>
   <si>
-    <t>This should be addressed through the projects.</t>
-  </si>
-  <si>
     <t>This is a secondary proposal form that is issued to do new projects based in a working group. Is it domain project or WG??</t>
   </si>
   <si>
@@ -1724,27 +1649,15 @@
     <t xml:space="preserve">TO DO </t>
   </si>
   <si>
-    <t>Person, vivo:orchidId URI (range is a resource)</t>
-  </si>
-  <si>
     <t>Person, foaf:homePage, URI (range is a resource)</t>
   </si>
   <si>
-    <t xml:space="preserve">REMOVED: This feature is not finally required after agreement in meetings. </t>
-  </si>
-  <si>
     <t>REMOVED: This was a misunderstanding, it wasn't a requirement</t>
   </si>
   <si>
     <t>Should be dcterms:contributor</t>
   </si>
   <si>
-    <t>move to roles</t>
-  </si>
-  <si>
-    <t>What type of publication</t>
-  </si>
-  <si>
     <t>Person, hasConflict, Conflict</t>
   </si>
   <si>
@@ -1760,39 +1673,9 @@
     <t>We don't reuse bibo because it adds a level of complexity</t>
   </si>
   <si>
-    <t>ENIGMAPublication is a bibo:AcademicArticle. Also may be bibo:Issue, bibo:Proceedings</t>
-  </si>
-  <si>
-    <t>ENIGMAPublication hasVenue, [string]</t>
-  </si>
-  <si>
-    <t>ENIGMAPublication dcterms:identifier, [string]</t>
-  </si>
-  <si>
-    <t>ENIGMAPublication  http://purl.org/dc/terms/date, [date]</t>
-  </si>
-  <si>
-    <t>ENIGMAPublication , http://purl.org/dc/terms/spatial, string</t>
-  </si>
-  <si>
     <t>change to hasProjectBriefDescription</t>
   </si>
   <si>
-    <t>ENIGMAPublication, bibo:DocumentStatus (it has a limited set ofinstances)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ENIGMAPublication, http://purl.org/dc/terms/title</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ENIGMAPublication, http://purl.org/dc/terms/contributor</t>
-  </si>
-  <si>
-    <t>Person, isPrincipalInvestigatorOf, Cohort</t>
-  </si>
-  <si>
-    <t>Person, isMainPrincipalInvestigatorOf, Cohort</t>
-  </si>
-  <si>
     <t>moved to roles</t>
   </si>
   <si>
@@ -1805,9 +1688,6 @@
     <t xml:space="preserve">Person, currentJobTitle, string [examples: student, postdoc, faculty, staff]. </t>
   </si>
   <si>
-    <t>should add the 4 types in the definition</t>
-  </si>
-  <si>
     <t>Person, hasGrant, string</t>
   </si>
   <si>
@@ -1832,7 +1712,229 @@
     <t>P39</t>
   </si>
   <si>
-    <t>should be subprop of http://purl.org/dc/terms/contributor</t>
+    <t>hasAffiliate is subproperty of foaf:hasMember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMOVED: This requirement is not finally required after agreement in meetings. </t>
+  </si>
+  <si>
+    <t>Person, hasResearchInterest, [string]</t>
+  </si>
+  <si>
+    <t>Describing the website of a person</t>
+  </si>
+  <si>
+    <t>Seee P42. This requirement was referring to job title. It is refined and captured there</t>
+  </si>
+  <si>
+    <t>Project, dc:contributor Person</t>
+  </si>
+  <si>
+    <t>vivo:Department, hasAffiliate, Person</t>
+  </si>
+  <si>
+    <t>AcademicArticle, bibo:DocumentStatus (it has a limited set ofinstances)</t>
+  </si>
+  <si>
+    <t>AcademicArticle, author, Person</t>
+  </si>
+  <si>
+    <t>we created enigma:Person, equivalent to foaf:Person, to address these requirements</t>
+  </si>
+  <si>
+    <t>Person, foaf:mbox, URI (range is a resource)</t>
+  </si>
+  <si>
+    <t>QualifiedAffiliation, hasStatus, {"Active" , "Inactive" , "Left Organization"}</t>
+  </si>
+  <si>
+    <t>QualifiedAffiliation, hasStartDate, [date]</t>
+  </si>
+  <si>
+    <t>QualifiedAffiliation, hasEndDate [date]</t>
+  </si>
+  <si>
+    <t>See P19</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, vcard:Address</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, vcard:Address, vcard:street-address, [string]</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, vcard:Address, vcard:region, [string]</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, vcard:Address,</t>
+  </si>
+  <si>
+    <t>hasPrimaryAddress is a subproperty of vcard:hasAddress</t>
+  </si>
+  <si>
+    <t>Could be described using vcard:hasAddress</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, vcard:Address, vcard:country-name, [string]</t>
+  </si>
+  <si>
+    <t>Person, hasPrimaryAddress, vcard:Address, vcard:postal-code, [string]</t>
+  </si>
+  <si>
+    <t>Person, vivo:orchidId, URI (range is a resource)</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>Project, dcterms:contributor, Person</t>
+  </si>
+  <si>
+    <t>moved to roles ontology</t>
+  </si>
+  <si>
+    <t>Describing the cohorts or projects a person is an ENIGMA contact of</t>
+  </si>
+  <si>
+    <t>[Cohort, Project] hasContact Person</t>
+  </si>
+  <si>
+    <t>Project, hasContact, Person</t>
+  </si>
+  <si>
+    <t>Pr27</t>
+  </si>
+  <si>
+    <t>Pr28</t>
+  </si>
+  <si>
+    <t>Pr29</t>
+  </si>
+  <si>
+    <t>Pr30</t>
+  </si>
+  <si>
+    <t>Pr31</t>
+  </si>
+  <si>
+    <t>Pr32</t>
+  </si>
+  <si>
+    <t>Pr33</t>
+  </si>
+  <si>
+    <t>Pr34</t>
+  </si>
+  <si>
+    <t>Pr35</t>
+  </si>
+  <si>
+    <t>Pr36</t>
+  </si>
+  <si>
+    <t>WorkingGroup, hasProject, Project, hasPublication, AcademicArticle</t>
+  </si>
+  <si>
+    <t>WorkingGroup, hasBriefDescription, [string]</t>
+  </si>
+  <si>
+    <t>WorkingGroup, dcterms:title, [string literal]</t>
+  </si>
+  <si>
+    <t>WorkingGroup, shortName, [string]</t>
+  </si>
+  <si>
+    <t>WorkingGroup, rdf:type, [HealthyVariation,  GeneticStudy, Methodology, ClinicalPopulation]</t>
+  </si>
+  <si>
+    <t>Project,hasDataAnalyst, Person</t>
+  </si>
+  <si>
+    <t>Project,hasGeneticDataAnalyst, Person</t>
+  </si>
+  <si>
+    <t>Project,hasImagingDataAnalyst, Person</t>
+  </si>
+  <si>
+    <t>Project,hasDataCollector, Person</t>
+  </si>
+  <si>
+    <t>Project,hasGeneticDataCollector, Person</t>
+  </si>
+  <si>
+    <t>Project,hasImagingDataCollector, Person</t>
+  </si>
+  <si>
+    <t>Project,hasDeveloper, Person</t>
+  </si>
+  <si>
+    <t>AcademicArticle, dcterms:contributor, author, Person</t>
+  </si>
+  <si>
+    <t>Project,hasDesigner, Person</t>
+  </si>
+  <si>
+    <t>AcademicArticle,hasReviewer, Person</t>
+  </si>
+  <si>
+    <t>AcademicArticle,firstDraftContributor, Person</t>
+  </si>
+  <si>
+    <t>AcademicArticle, http://purl.org/dc/terms/title</t>
+  </si>
+  <si>
+    <t>AcademicArticle, http://purl.org/dc/terms/contributor</t>
+  </si>
+  <si>
+    <t>AcademicArticle, hasVenue, [string]</t>
+  </si>
+  <si>
+    <t>AcademicArticle, dcterms:identifier, [string]</t>
+  </si>
+  <si>
+    <t>AcademicArticle,  http://purl.org/dc/terms/date, [date]</t>
+  </si>
+  <si>
+    <t>AcademicArticle, , http://purl.org/dc/terms/spatial, string</t>
+  </si>
+  <si>
+    <t>AcademicArticle, is a bibo:AcademicArticle. Also may be bibo:Issue, bibo:Proceedings</t>
+  </si>
+  <si>
+    <t>What type of publication is the current paper?</t>
+  </si>
+  <si>
+    <t>Cohort, hasPrincipalInvestigator, Person</t>
+  </si>
+  <si>
+    <t>Cohort, hasMainPrincipalInvestigator, Person</t>
   </si>
 </sst>
 </file>
@@ -2580,8 +2682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2596,18 +2698,18 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2616,12 +2718,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
@@ -2632,7 +2734,7 @@
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>22</v>
@@ -2643,7 +2745,7 @@
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -2654,7 +2756,7 @@
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
@@ -2665,7 +2767,7 @@
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
@@ -2676,7 +2778,7 @@
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
@@ -2687,7 +2789,7 @@
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
@@ -2698,7 +2800,7 @@
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
@@ -2709,7 +2811,7 @@
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>24</v>
@@ -2720,7 +2822,7 @@
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -2731,7 +2833,7 @@
     </row>
     <row r="15" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>27</v>
@@ -2740,12 +2842,12 @@
         <v>28</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>29</v>
@@ -2756,7 +2858,7 @@
     </row>
     <row r="17" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>31</v>
@@ -2767,7 +2869,7 @@
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>33</v>
@@ -2778,7 +2880,7 @@
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>35</v>
@@ -2789,7 +2891,7 @@
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>37</v>
@@ -2800,21 +2902,21 @@
     </row>
     <row r="21" spans="1:4" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>524</v>
+        <v>501</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>40</v>
@@ -2825,18 +2927,18 @@
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>46</v>
@@ -2847,7 +2949,7 @@
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>47</v>
@@ -2858,7 +2960,7 @@
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>48</v>
@@ -2869,7 +2971,7 @@
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
@@ -2880,7 +2982,7 @@
     </row>
     <row r="28" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>52</v>
@@ -2889,12 +2991,12 @@
         <v>53</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
@@ -2905,7 +3007,7 @@
     </row>
     <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>56</v>
@@ -2916,7 +3018,7 @@
     </row>
     <row r="31" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>58</v>
@@ -2925,12 +3027,12 @@
         <v>3</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>59</v>
@@ -2941,7 +3043,7 @@
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>61</v>
@@ -2952,7 +3054,7 @@
     </row>
     <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>63</v>
@@ -2963,7 +3065,7 @@
     </row>
     <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>65</v>
@@ -2974,7 +3076,7 @@
     </row>
     <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>67</v>
@@ -2985,7 +3087,7 @@
     </row>
     <row r="37" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>69</v>
@@ -2994,12 +3096,12 @@
         <v>70</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>71</v>
@@ -3008,12 +3110,12 @@
         <v>72</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>73</v>
@@ -3022,12 +3124,12 @@
         <v>74</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>75</v>
@@ -3036,507 +3138,507 @@
         <v>76</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>114</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B83" s="5" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>556</v>
+        <v>531</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B84" s="5" t="s">
-        <v>554</v>
+        <v>529</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>556</v>
+        <v>531</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B85" s="5" t="s">
-        <v>555</v>
+        <v>530</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>556</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -3554,8 +3656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3569,12 +3671,12 @@
         <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>543</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3583,12 +3685,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3599,396 +3701,426 @@
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>118</v>
+      <c r="C5" s="5" t="s">
+        <v>587</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>561</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>120</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>122</v>
+        <v>449</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>124</v>
+        <v>360</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>126</v>
+        <v>361</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>124</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>128</v>
+        <v>362</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>130</v>
+        <v>363</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>128</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>132</v>
+        <v>364</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>134</v>
+        <v>365</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>562</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>546</v>
+        <v>521</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>574</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>529</v>
+        <v>505</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>565</v>
+        <v>536</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>530</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>592</v>
+      </c>
       <c r="B30" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A31" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="D31" t="s">
         <v>538</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B31" s="5" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A32" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A33" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A35" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="D35" t="s">
         <v>539</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>566</v>
-      </c>
-      <c r="D31" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B32" s="5" t="s">
-        <v>547</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B33" s="5" t="s">
-        <v>548</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B34" s="5" t="s">
-        <v>549</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B35" s="5" t="s">
-        <v>550</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>570</v>
-      </c>
-      <c r="D35" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A36" s="17" t="s">
+        <v>598</v>
+      </c>
       <c r="B36" s="5" t="s">
-        <v>551</v>
+        <v>526</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A37" s="17" t="s">
+        <v>599</v>
+      </c>
       <c r="B37" s="5" t="s">
-        <v>552</v>
+        <v>527</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A38" s="17" t="s">
+        <v>600</v>
+      </c>
       <c r="B38" s="5" t="s">
-        <v>553</v>
+        <v>528</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A39" s="17" t="s">
+        <v>601</v>
+      </c>
       <c r="B39" s="17" t="s">
-        <v>563</v>
+        <v>625</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>569</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -4006,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4018,15 +4150,15 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C1" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4035,134 +4167,137 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -4180,26 +4315,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.296875" customWidth="1"/>
-    <col min="3" max="3" width="90.796875" customWidth="1"/>
+    <col min="3" max="3" width="77.296875" customWidth="1"/>
     <col min="4" max="4" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4208,550 +4343,560 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>218</v>
+        <v>215</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>581</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>580</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>580</v>
+        <v>541</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>580</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>580</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>580</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>580</v>
+        <v>541</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>593</v>
+        <v>229</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>497</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>446</v>
+        <v>400</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>589</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>242</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>578</v>
+        <v>626</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>579</v>
+        <v>627</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D21" t="s">
-        <v>560</v>
+        <v>533</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>447</v>
+        <v>240</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>500</v>
+        <v>244</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D28" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>259</v>
+        <v>555</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>517</v>
+        <v>415</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>261</v>
+        <v>556</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>510</v>
+        <v>488</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>511</v>
+        <v>489</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>503</v>
+        <v>486</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>506</v>
+        <v>484</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>587</v>
+        <v>547</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>507</v>
+        <v>485</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>588</v>
+        <v>548</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>447</v>
+        <v>437</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>589</v>
+        <v>549</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>450</v>
+        <v>436</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>590</v>
+        <v>550</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>452</v>
+        <v>438</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>591</v>
+        <v>551</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>454</v>
+        <v>439</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>592</v>
+        <v>552</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>458</v>
+        <v>440</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>457</v>
+        <v>441</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A45" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>583</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>584</v>
+        <v>444</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>513</v>
+        <v>491</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>509</v>
+        <v>487</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>512</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>514</v>
+        <v>492</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A49" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>586</v>
+        <v>494</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>545</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4804,7 +4949,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4816,12 +4961,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4830,26 +4975,26 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -4857,118 +5002,115 @@
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>518</v>
+        <v>496</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>545</v>
+        <v>264</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>540</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>519</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>520</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>523</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>522</v>
+        <v>267</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>521</v>
+        <v>499</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>527</v>
+        <v>503</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>528</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -4982,6 +5124,183 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="59.09765625" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="B1" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="17" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>508</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>509</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>577</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>511</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>607</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>583</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>610</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A12" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A13" s="17" t="s">
+        <v>585</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A14" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -4998,20 +5317,20 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5020,102 +5339,102 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -5131,140 +5450,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="B1" s="1" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>465</v>
-      </c>
-      <c r="C2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>532</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>533</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>468</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12" t="s">
-        <v>535</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12" t="s">
-        <v>536</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B12" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B13" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B14" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B18" s="5" t="s">
-        <v>537</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
minor updates on reqs
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirments.xlsx
+++ b/requirements/Enigma_requirments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -1565,9 +1565,6 @@
     <t>Secondary Proposal Form</t>
   </si>
   <si>
-    <t>Is this needed?</t>
-  </si>
-  <si>
     <t>What is the publication of a project?</t>
   </si>
   <si>
@@ -1935,6 +1932,9 @@
   </si>
   <si>
     <t>Cohort, hasMainPrincipalInvestigator, Person</t>
+  </si>
+  <si>
+    <t>This is for a project, not a WG</t>
   </si>
 </sst>
 </file>
@@ -3622,23 +3622,23 @@
         <v>459</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B84" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B85" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="C85" s="12" t="s">
         <v>530</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -3656,7 +3656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -3671,7 +3671,7 @@
         <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
@@ -3707,10 +3707,10 @@
         <v>117</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3721,7 +3721,7 @@
         <v>118</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3735,7 +3735,7 @@
         <v>120</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3749,7 +3749,7 @@
         <v>122</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3763,7 +3763,7 @@
         <v>124</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3777,7 +3777,7 @@
         <v>126</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3791,7 +3791,7 @@
         <v>128</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3805,7 +3805,7 @@
         <v>130</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3819,7 +3819,7 @@
         <v>132</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3921,7 +3921,7 @@
         <v>150</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3946,7 +3946,7 @@
         <v>154</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -3995,132 +3995,132 @@
     </row>
     <row r="29" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>536</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C31" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="D31" t="s">
         <v>537</v>
-      </c>
-      <c r="D31" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -4181,7 +4181,7 @@
         <v>204</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4315,7 +4315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -4354,10 +4354,10 @@
         <v>215</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4371,7 +4371,7 @@
         <v>217</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4385,7 +4385,7 @@
         <v>219</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4399,7 +4399,7 @@
         <v>220</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4413,7 +4413,7 @@
         <v>226</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4427,7 +4427,7 @@
         <v>227</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4441,7 +4441,7 @@
         <v>228</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4455,7 +4455,7 @@
         <v>230</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4488,7 +4488,7 @@
         <v>232</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D14" s="17"/>
     </row>
@@ -4500,7 +4500,7 @@
         <v>234</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4519,10 +4519,10 @@
         <v>400</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>588</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>589</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4544,7 +4544,7 @@
         <v>236</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4555,7 +4555,7 @@
         <v>237</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4569,7 +4569,7 @@
         <v>239</v>
       </c>
       <c r="D21" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4583,7 +4583,7 @@
         <v>493</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4627,7 +4627,7 @@
         <v>244</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4652,7 +4652,7 @@
         <v>247</v>
       </c>
       <c r="D28" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4686,7 +4686,7 @@
         <v>251</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4700,7 +4700,7 @@
         <v>495</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4708,10 +4708,10 @@
         <v>416</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4733,7 +4733,7 @@
         <v>486</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4744,79 +4744,79 @@
         <v>484</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>485</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>437</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>436</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>438</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>439</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>440</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4827,7 +4827,7 @@
         <v>441</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4838,7 +4838,7 @@
         <v>444</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4846,10 +4846,10 @@
         <v>478</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4882,7 +4882,7 @@
         <v>494</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4890,13 +4890,13 @@
         <v>502</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C49" s="17" t="s">
+        <v>544</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>545</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -4948,8 +4948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5033,7 +5033,7 @@
         <v>496</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -5044,7 +5044,7 @@
         <v>264</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -5066,7 +5066,7 @@
         <v>267</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -5074,10 +5074,10 @@
         <v>428</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -5085,10 +5085,10 @@
         <v>497</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -5099,7 +5099,7 @@
         <v>500</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
@@ -5110,7 +5110,7 @@
         <v>503</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>504</v>
+        <v>627</v>
       </c>
     </row>
   </sheetData>
@@ -5167,132 +5167,132 @@
     </row>
     <row r="4" spans="1:4" s="17" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>509</v>
-      </c>
       <c r="C4" s="17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>216</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>218</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>224</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>221</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>222</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>223</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>225</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>